<commit_message>
Completed translation of Town ★8 quest information. Investigate additional crawl targets : G★2 ~ G★4 quest
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18920"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3505" uniqueCount="1149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3552" uniqueCount="1184">
   <si>
     <t>questName</t>
   </si>
@@ -64,7 +64,7 @@
     <t>50분</t>
   </si>
   <si>
-    <t>불로나방(不老蛾) 3마리 납품</t>
+    <t>불로아(不老蛾) 3마리 납품</t>
   </si>
   <si>
     <t>부나하부라(ブナハブラ) 3마리 토벌</t>
@@ -2923,409 +2923,514 @@
     <t>마을★8</t>
   </si>
   <si>
-    <t>タイムアップもしくはネコタクチケットの納品</t>
-  </si>
-  <si>
     <t>竜の卵の納品・ランチ</t>
   </si>
   <si>
+    <t>용의 알 납품・런치</t>
+  </si>
+  <si>
+    <t>밀림(密林)</t>
+  </si>
+  <si>
+    <t>氷海の採集ツアー</t>
+  </si>
+  <si>
+    <t>빙해 채집 투어</t>
+  </si>
+  <si>
+    <t>빙해(氷海)</t>
+  </si>
+  <si>
+    <t>龍識船強化！【溶岩竜編】</t>
+  </si>
+  <si>
+    <t>용식선강화! [용암룡편]</t>
+  </si>
+  <si>
+    <t>볼가노스(ヴォルガノス) 1마리 수렵</t>
+  </si>
+  <si>
+    <t>珍肥料を手に入れるのニャ！</t>
+  </si>
+  <si>
+    <t>진비료를 손에 넣는거다냐!</t>
+  </si>
+  <si>
+    <t>불로아(不老蛾) 10마리 납품</t>
+  </si>
+  <si>
+    <t>영원의 화석(久遠の化石) 1개 납품</t>
+  </si>
+  <si>
+    <t>ナイショのお仕事</t>
+  </si>
+  <si>
+    <t>비밀스런 일</t>
+  </si>
+  <si>
+    <t>초식룡의 알(草食竜の卵) 2개 납품</t>
+  </si>
+  <si>
+    <t>たまには釣りでもいかが？</t>
+  </si>
+  <si>
+    <t>가끔씩은 낚시라도 하는게 어때?</t>
+  </si>
+  <si>
+    <t>가노토토스(ガノトトス) 1마리 수렵</t>
+  </si>
+  <si>
+    <t>宣伝ネコの受難</t>
+  </si>
+  <si>
+    <t>선전고양이의 수난</t>
+  </si>
+  <si>
+    <t>가라라아쟈라(ガララアジャラ) 1마리 수렵</t>
+  </si>
+  <si>
+    <t>가라라아쟈라(ガララアジャラ)의 머리 파괴</t>
+  </si>
+  <si>
+    <t>7800z</t>
+  </si>
+  <si>
+    <t>なんと、黒狼鳥でした！</t>
+  </si>
+  <si>
+    <t>무려, 흑랑조였습니다!</t>
+  </si>
+  <si>
+    <t>얀가루루가(イャンガルルガ)의 머리 파괴</t>
+  </si>
+  <si>
+    <t>冷血なるドスギアノス！</t>
+  </si>
+  <si>
+    <t>냉혈한 도스기아노스!</t>
+  </si>
+  <si>
+    <t>도스기아노스(ドスギアノス) 2마리 수렵</t>
+  </si>
+  <si>
+    <t>龍識船強化！【迅竜編】</t>
+  </si>
+  <si>
+    <t>욕식선강화! [신룡편]</t>
+  </si>
+  <si>
+    <t>나루가크루가(ナルガクルガ) 1마리 수렵</t>
+  </si>
+  <si>
+    <t>密林の採集ツアー</t>
+  </si>
+  <si>
+    <t>밀림 채집 투어</t>
+  </si>
+  <si>
+    <t>火山の厄介者たち</t>
+  </si>
+  <si>
+    <t>화산의 골칫거리들</t>
+  </si>
+  <si>
+    <t>바살모스(バサルモス) 1마리와 도스이오스(ドスイーオス) 1마리 수렵</t>
+  </si>
+  <si>
+    <t>道化師は斯く嘲る</t>
+  </si>
+  <si>
+    <t>광대는 이렇게 비웃는다</t>
+  </si>
+  <si>
+    <t>호로로호루루(ホロロホルル)의 꼬리 파괴</t>
+  </si>
+  <si>
+    <t>熱地に現る、ウラガンキン！</t>
+  </si>
+  <si>
+    <t>열대에 나타나다, 우라간킨!</t>
+  </si>
+  <si>
+    <t>우라간킨(ウラガンキン)의 꼬리 절단</t>
+  </si>
+  <si>
+    <t>ものぐさには爆鎚竜で喝！</t>
+  </si>
+  <si>
+    <t>게으름뱅이에게는 폭추룡으로 갈!</t>
+  </si>
+  <si>
+    <t>지저화산(地底火山)</t>
+  </si>
+  <si>
+    <t>でっかい岩だと思ったら…？</t>
+  </si>
+  <si>
+    <t>커다란 바위라고 생각했더니...?</t>
+  </si>
+  <si>
+    <t>바살모스(バサルモス) 1마리 수렵</t>
+  </si>
+  <si>
+    <t>飛んで跳ねて無我夢中</t>
+  </si>
+  <si>
+    <t>날고 뛰어오르며 무아무중</t>
+  </si>
+  <si>
+    <t>케챠와챠(ケチャワチャ) 1마리와 도스마콰(ドスマッカォ) 1마리 수렵</t>
+  </si>
+  <si>
+    <t>砂まみれですな</t>
+  </si>
+  <si>
+    <t>모래투성이군요</t>
+  </si>
+  <si>
+    <t>하플봇카(ハプルボッカ) 1마리와 도스가레오스(ドスガレオス) 1마리 수렵</t>
+  </si>
+  <si>
+    <t>沼地の恐怖体験</t>
+  </si>
+  <si>
+    <t>늪지의 공포체험</t>
+  </si>
+  <si>
+    <t>쇼군기자미(ショウグンギザミ) 1마리와 바바콩가(ババコンガ) 1마리 수렵</t>
+  </si>
+  <si>
+    <t>陸の女王、捕獲作戦！</t>
+  </si>
+  <si>
+    <t>육지의 여왕, 포획작전!</t>
+  </si>
+  <si>
+    <t>리오레이아(リオレイア) 1마리 포획</t>
+  </si>
+  <si>
+    <t>喰われる前にヤレ！</t>
+  </si>
+  <si>
+    <t>먹히기 전에 해치워라!</t>
+  </si>
+  <si>
+    <t>하플봇카(ハプルボッカ)의 아가미 파괴</t>
+  </si>
+  <si>
+    <t>狩人のための舞台～氷海～</t>
+  </si>
+  <si>
+    <t>사냥꾼을 위한 무대 ~빙해~</t>
+  </si>
+  <si>
+    <t>푸르푸르(フルフル) 1마리 수렵</t>
+  </si>
+  <si>
+    <t>스쿠아길(スクアギル) 6마리 토벌</t>
+  </si>
+  <si>
+    <t>山嶺を舞うリオレイア</t>
+  </si>
+  <si>
+    <t>산봉우리에서 춤추는 리오레이아</t>
+  </si>
+  <si>
+    <t>転がれ！転がせ！赤い牙獣</t>
+  </si>
+  <si>
+    <t>굴러라! 굴려라! 붉은 아수</t>
+  </si>
+  <si>
+    <t>랑그로토라(ラングロトラ)의 등 파괴</t>
+  </si>
+  <si>
+    <t>原生林に巣食う蜘蛛</t>
+  </si>
+  <si>
+    <t>원시림에 둥지를 튼 거미</t>
+  </si>
+  <si>
+    <t>네르스큐라(ネルスキュラ) 1마리 수렵</t>
+  </si>
+  <si>
+    <t>おやつは高層エリンギ</t>
+  </si>
+  <si>
+    <t>간식은 고층새송이버섯</t>
+  </si>
+  <si>
+    <t>고층새송이버섯(高層エリンギ) 10개 납품</t>
+  </si>
+  <si>
+    <t>はじける貝殻マネー</t>
+  </si>
+  <si>
+    <t>여물어서 터지는 조개 껍데기 흉내</t>
+  </si>
+  <si>
+    <t>예쁜 조개껍데기(きれいな貝殻) 10개 납품</t>
+  </si>
+  <si>
+    <t>블루팡고(ブルファンゴ) 8마리 토벌</t>
+  </si>
+  <si>
+    <t>龍識船強化！【水竜編】</t>
+  </si>
+  <si>
+    <t>용식선강화! [수룡편]</t>
+  </si>
+  <si>
+    <t>ホワイトアウト</t>
+  </si>
+  <si>
+    <t>화이트 아웃</t>
+  </si>
+  <si>
+    <t>블랑고(ブランゴ) 6마리 토벌</t>
+  </si>
+  <si>
+    <t>美しき、遺群嶺</t>
+  </si>
+  <si>
+    <t>아름다운 유군령</t>
+  </si>
+  <si>
+    <t>쿤츄(クンチュウ)와 오르타로스(オルタロス) 합계 20마리 토벌</t>
+  </si>
+  <si>
+    <t>切り裂かれた誇り</t>
+  </si>
+  <si>
+    <t>찢어발겨진 긍지</t>
+  </si>
+  <si>
+    <t>地底火山の採集ツアー</t>
+  </si>
+  <si>
+    <t>지저화산 채집 투어</t>
+  </si>
+  <si>
+    <t>ナルガクルガのお手本</t>
+  </si>
+  <si>
+    <t>나루가크루가의 본보기</t>
+  </si>
+  <si>
+    <t>루도로스(ルドロス) 6마리 토벌</t>
+  </si>
+  <si>
+    <t>ぷくぅーっ！ザボアザギル！</t>
+  </si>
+  <si>
+    <t>퓨우웃! 자보아자길</t>
+  </si>
+  <si>
+    <t>자보아자길(ザボアザギル) 1마리 수렵</t>
+  </si>
+  <si>
+    <t>자보아자길(ザボアザギル)의 머리 파과</t>
+  </si>
+  <si>
+    <t>雷光の先の面影</t>
+  </si>
+  <si>
+    <t>뇌광 앞의 모습</t>
+  </si>
+  <si>
+    <t>대뇌광충(大雷光虫) 15마리 토벌</t>
+  </si>
+  <si>
+    <t>フルフルのまごころ診療所</t>
+  </si>
+  <si>
+    <t>푸르푸르의 진심 진료소</t>
+  </si>
+  <si>
+    <t>푸르푸르(フルフル)의 몸통 파괴</t>
+  </si>
+  <si>
+    <t>桃毛獣のトサカ破壊に挑戦！</t>
+  </si>
+  <si>
+    <t>도모수의 볏 파괴 도전!</t>
+  </si>
+  <si>
+    <t>嗚呼素晴らしき也、絞蛇竜</t>
+  </si>
+  <si>
+    <t>아아 훌륭하도다, 교사룡</t>
+  </si>
+  <si>
+    <t>가라라아쟈라(ガララアジャラ) 1마리 포획</t>
+  </si>
+  <si>
+    <t>孤島からの伝書</t>
+  </si>
+  <si>
+    <t>고도로부터의 전서</t>
+  </si>
+  <si>
+    <t>호로로호루루(ホロロホルル) 1마리와 테츠카브라(テツカブラ) 1마리 수렵</t>
+  </si>
+  <si>
+    <t>轟竜の狩猟をさせてやるぜ！</t>
+  </si>
+  <si>
+    <t>굉룡 수렵을 시켜주지!</t>
+  </si>
+  <si>
+    <t>마을★9</t>
+  </si>
+  <si>
+    <t>ティガレックスの尻尾切断</t>
+  </si>
+  <si>
+    <t>ライゼクス、再び！</t>
+  </si>
+  <si>
+    <t>라이젝스, 다시한번!</t>
+  </si>
+  <si>
+    <t>ライゼクス１頭の狩猟</t>
+  </si>
+  <si>
+    <t>龍識船強化！【氷牙竜編】</t>
+  </si>
+  <si>
+    <t>용식선강화! [빙아룡편]</t>
+  </si>
+  <si>
+    <t>ベリオロス１頭の狩猟</t>
+  </si>
+  <si>
+    <t>タマミツネ、再び！</t>
+  </si>
+  <si>
+    <t>타마미츠네, 다시한번!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">タマミツネ１頭の狩猟 </t>
+  </si>
+  <si>
+    <t>騎士と古代林の挑戦</t>
+  </si>
+  <si>
+    <t>기사와 고대림의 도전</t>
+  </si>
+  <si>
+    <t>キリンの討伐</t>
+  </si>
+  <si>
+    <t>ガムートの強さは世界一</t>
+  </si>
+  <si>
+    <t>ガムート１頭の捕獲</t>
+  </si>
+  <si>
+    <t>ガムートの頭部破壊</t>
+  </si>
+  <si>
+    <t>11400z</t>
+  </si>
+  <si>
+    <t>嗚呼素晴らしき也、雷狼竜</t>
+  </si>
+  <si>
+    <t>ジンオウガ１頭の捕獲</t>
+  </si>
+  <si>
+    <t>ガブラス５頭の討伐</t>
+  </si>
+  <si>
+    <t>犯人はキミだ、雷狼竜</t>
+  </si>
+  <si>
+    <t>ジンオウガの頭部破壊</t>
+  </si>
+  <si>
+    <t>突撃取材！巨大甲虫を追え！</t>
+  </si>
+  <si>
+    <t>ゲネル・セルタス１匹の狩猟</t>
+  </si>
+  <si>
+    <t>ゲネル・セルタスの尻尾破壊</t>
+  </si>
+  <si>
+    <t>氷海に君臨する者</t>
+  </si>
+  <si>
+    <t>割り込み受注：卵納品</t>
+  </si>
+  <si>
     <t>竜の卵２個の納品</t>
   </si>
   <si>
-    <t>リオレイア１頭の狩猟</t>
-  </si>
-  <si>
-    <t>氷海の採集ツアー</t>
-  </si>
-  <si>
-    <t>龍識船強化！【溶岩竜編】</t>
-  </si>
-  <si>
-    <t>ヴォルガノス１頭の狩猟</t>
-  </si>
-  <si>
-    <t>珍肥料を手に入れるのニャ！</t>
-  </si>
-  <si>
-    <t>不老蛾１０匹の納品</t>
-  </si>
-  <si>
-    <t>久遠の化石１個の納品</t>
-  </si>
-  <si>
-    <t>ナイショのお仕事</t>
-  </si>
-  <si>
-    <t>たまには釣りでもいかが？</t>
-  </si>
-  <si>
-    <t>黄金魚３匹の納品</t>
-  </si>
-  <si>
-    <t>ガノトトス１頭の狩猟</t>
-  </si>
-  <si>
-    <t>宣伝ネコの受難</t>
-  </si>
-  <si>
-    <t>ガララアジャラ１頭の狩猟</t>
-  </si>
-  <si>
-    <t>ガララアジャラの頭部破壊</t>
-  </si>
-  <si>
-    <t>7800z</t>
-  </si>
-  <si>
-    <t>なんと、黒狼鳥でした！</t>
-  </si>
-  <si>
-    <t>イャンガルルガ１頭の狩猟</t>
-  </si>
-  <si>
-    <t>イャンガルルガの頭部破壊</t>
-  </si>
-  <si>
-    <t>冷血なるドスギアノス！</t>
-  </si>
-  <si>
-    <t>ドスギアノス２頭の狩猟</t>
-  </si>
-  <si>
-    <t>龍識船強化！【迅竜編】</t>
-  </si>
-  <si>
-    <t>ナルガクルガ１頭の狩猟</t>
-  </si>
-  <si>
-    <t>密林の採集ツアー</t>
-  </si>
-  <si>
-    <t>火山の厄介者たち</t>
-  </si>
-  <si>
-    <t>バサルモス１頭とドスイーオス１頭の狩猟</t>
-  </si>
-  <si>
-    <t>道化師は斯く嘲る</t>
-  </si>
-  <si>
-    <t>ホロロホルル１頭の狩猟</t>
-  </si>
-  <si>
-    <t>ホロロホルルの尻尾破壊</t>
-  </si>
-  <si>
-    <t>熱地に現る、ウラガンキン！</t>
-  </si>
-  <si>
-    <t>ウラガンキン１頭の狩猟</t>
-  </si>
-  <si>
-    <t>ウラガンキンの尻尾切断</t>
-  </si>
-  <si>
-    <t>ものぐさには爆鎚竜で喝！</t>
-  </si>
-  <si>
-    <t>でっかい岩だと思ったら…？</t>
-  </si>
-  <si>
-    <t>バサルモス１頭の狩猟</t>
-  </si>
-  <si>
-    <t>飛んで跳ねて無我夢中</t>
-  </si>
-  <si>
-    <t>ケチャワチャ１頭とドスマッカォ１頭の狩猟</t>
+    <t>轟竜と赤甲獣のデュエット</t>
+  </si>
+  <si>
+    <t>ティガレックス１頭とラングロトラ１頭の狩猟</t>
+  </si>
+  <si>
+    <t>10500z</t>
+  </si>
+  <si>
+    <t>アグナコトルの捕獲</t>
+  </si>
+  <si>
+    <t>アグナコトル１頭の捕獲</t>
+  </si>
+  <si>
+    <t>ウロコトル５頭の討伐</t>
+  </si>
+  <si>
+    <t>火山の迷惑集団襲来！</t>
+  </si>
+  <si>
+    <t>古代林の大運動会</t>
+  </si>
+  <si>
+    <t>9300z</t>
+  </si>
+  <si>
+    <t>鎧竜は、とってもグルメ？</t>
+  </si>
+  <si>
+    <t>グラビモス１頭の狩猟</t>
+  </si>
+  <si>
+    <t>グラビモスの頭部破壊</t>
+  </si>
+  <si>
+    <t>凶運の遺跡平原</t>
+  </si>
+  <si>
+    <t>乗りによるダウンを４回成功</t>
+  </si>
+  <si>
+    <t>美しき幻獣</t>
+  </si>
+  <si>
+    <t>遺群嶺の火竜</t>
+  </si>
+  <si>
+    <t>リオレウスの翼破壊</t>
+  </si>
+  <si>
+    <t>海竜、沈降開始</t>
+  </si>
+  <si>
+    <t>ラギアクルス１頭の狩猟</t>
+  </si>
+  <si>
+    <t>雪山、雪玉、雪合戦！！</t>
+  </si>
+  <si>
+    <t>ドドブランゴ１頭とウルクスス１頭の狩猟</t>
   </si>
   <si>
     <t>龍歴院ポイント５００pts入手</t>
-  </si>
-  <si>
-    <t>砂まみれですな</t>
-  </si>
-  <si>
-    <t>ハプルボッカ１頭とドスガレオス１頭の狩猟</t>
-  </si>
-  <si>
-    <t>沼地の恐怖体験</t>
-  </si>
-  <si>
-    <t>ショウグンギザミ１匹とババコンガ１頭の狩猟</t>
-  </si>
-  <si>
-    <t>陸の女王、捕獲作戦！</t>
-  </si>
-  <si>
-    <t>リオレイア１頭の捕獲</t>
-  </si>
-  <si>
-    <t>喰われる前にヤレ！</t>
-  </si>
-  <si>
-    <t>ハプルボッカ１頭の狩猟</t>
-  </si>
-  <si>
-    <t>ハプルボッカのエラ破壊</t>
-  </si>
-  <si>
-    <t>狩人のための舞台～氷海～</t>
-  </si>
-  <si>
-    <t>フルフル１頭の狩猟</t>
-  </si>
-  <si>
-    <t>スクアギル６頭の討伐</t>
-  </si>
-  <si>
-    <t>山嶺を舞うリオレイア</t>
-  </si>
-  <si>
-    <t>リオレイアの尻尾切断</t>
-  </si>
-  <si>
-    <t>転がれ！転がせ！赤い牙獣</t>
-  </si>
-  <si>
-    <t>ラングロトラ１頭の狩猟</t>
-  </si>
-  <si>
-    <t>ラングロトラの背中破壊</t>
-  </si>
-  <si>
-    <t>原生林に巣食う蜘蛛</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ネルスキュラ１匹の狩猟 </t>
-  </si>
-  <si>
-    <t>おやつは高層エリンギ</t>
-  </si>
-  <si>
-    <t>高層エリンギ１０個の納品</t>
-  </si>
-  <si>
-    <t>はじける貝殻マネー</t>
-  </si>
-  <si>
-    <t>きれいな貝殻１０個の納品</t>
-  </si>
-  <si>
-    <t>ブルファンゴ８頭の討伐</t>
-  </si>
-  <si>
-    <t>龍識船強化！【水竜編】</t>
-  </si>
-  <si>
-    <t>ホワイトアウト</t>
-  </si>
-  <si>
-    <t>ドドブランゴ１頭の狩猟</t>
-  </si>
-  <si>
-    <t>ブランゴ６頭の討伐</t>
-  </si>
-  <si>
-    <t>美しき、遺群嶺</t>
-  </si>
-  <si>
-    <t>クンチュウとオルタロス合計２０匹の討伐</t>
-  </si>
-  <si>
-    <t>切り裂かれた誇り</t>
-  </si>
-  <si>
-    <t>ショウグンギザミ１匹の狩猟</t>
-  </si>
-  <si>
-    <t>ショウグンギザミのヤド破壊</t>
-  </si>
-  <si>
-    <t>地底火山の採集ツアー</t>
-  </si>
-  <si>
-    <t>ナルガクルガのお手本</t>
-  </si>
-  <si>
-    <t>ルドロス５頭の討伐</t>
-  </si>
-  <si>
-    <t>ぷくぅーっ！ザボアザギル！</t>
-  </si>
-  <si>
-    <t>ザボアザギル１頭の狩猟</t>
-  </si>
-  <si>
-    <t>ザボアザギルの頭部破壊</t>
-  </si>
-  <si>
-    <t>雷光の先の面影</t>
-  </si>
-  <si>
-    <t>大雷光虫１５匹の討伐</t>
-  </si>
-  <si>
-    <t>フルフルのまごころ診療所</t>
-  </si>
-  <si>
-    <t>フルフルの胴体破壊</t>
-  </si>
-  <si>
-    <t>桃毛獣のトサカ破壊に挑戦！</t>
-  </si>
-  <si>
-    <t>ババコンガのトサカ破壊</t>
-  </si>
-  <si>
-    <t>嗚呼素晴らしき也、絞蛇竜</t>
-  </si>
-  <si>
-    <t>ガララアジャラ１頭の捕獲</t>
-  </si>
-  <si>
-    <t>孤島からの伝書</t>
-  </si>
-  <si>
-    <t>ホロロホルル１頭とテツカブラ１頭の狩猟</t>
-  </si>
-  <si>
-    <t>轟竜の狩猟をさせてやるぜ！</t>
-  </si>
-  <si>
-    <t>마을★9</t>
-  </si>
-  <si>
-    <t>ティガレックスの尻尾切断</t>
-  </si>
-  <si>
-    <t>ライゼクス、再び！</t>
-  </si>
-  <si>
-    <t>ライゼクス１頭の狩猟</t>
-  </si>
-  <si>
-    <t>龍識船強化！【氷牙竜編】</t>
-  </si>
-  <si>
-    <t>ベリオロス１頭の狩猟</t>
-  </si>
-  <si>
-    <t>タマミツネ、再び！</t>
-  </si>
-  <si>
-    <t xml:space="preserve">タマミツネ１頭の狩猟 </t>
-  </si>
-  <si>
-    <t>騎士と古代林の挑戦</t>
-  </si>
-  <si>
-    <t>キリンの討伐</t>
-  </si>
-  <si>
-    <t>ガムートの強さは世界一</t>
-  </si>
-  <si>
-    <t>ガムート１頭の捕獲</t>
-  </si>
-  <si>
-    <t>ガムートの頭部破壊</t>
-  </si>
-  <si>
-    <t>11400z</t>
-  </si>
-  <si>
-    <t>嗚呼素晴らしき也、雷狼竜</t>
-  </si>
-  <si>
-    <t>ジンオウガ１頭の捕獲</t>
-  </si>
-  <si>
-    <t>ガブラス５頭の討伐</t>
-  </si>
-  <si>
-    <t>犯人はキミだ、雷狼竜</t>
-  </si>
-  <si>
-    <t>ジンオウガの頭部破壊</t>
-  </si>
-  <si>
-    <t>突撃取材！巨大甲虫を追え！</t>
-  </si>
-  <si>
-    <t>ゲネル・セルタス１匹の狩猟</t>
-  </si>
-  <si>
-    <t>ゲネル・セルタスの尻尾破壊</t>
-  </si>
-  <si>
-    <t>氷海に君臨する者</t>
-  </si>
-  <si>
-    <t>割り込み受注：卵納品</t>
-  </si>
-  <si>
-    <t>轟竜と赤甲獣のデュエット</t>
-  </si>
-  <si>
-    <t>ティガレックス１頭とラングロトラ１頭の狩猟</t>
-  </si>
-  <si>
-    <t>10500z</t>
-  </si>
-  <si>
-    <t>アグナコトルの捕獲</t>
-  </si>
-  <si>
-    <t>アグナコトル１頭の捕獲</t>
-  </si>
-  <si>
-    <t>ウロコトル５頭の討伐</t>
-  </si>
-  <si>
-    <t>火山の迷惑集団襲来！</t>
-  </si>
-  <si>
-    <t>古代林の大運動会</t>
-  </si>
-  <si>
-    <t>9300z</t>
-  </si>
-  <si>
-    <t>鎧竜は、とってもグルメ？</t>
-  </si>
-  <si>
-    <t>グラビモス１頭の狩猟</t>
-  </si>
-  <si>
-    <t>グラビモスの頭部破壊</t>
-  </si>
-  <si>
-    <t>凶運の遺跡平原</t>
-  </si>
-  <si>
-    <t>乗りによるダウンを４回成功</t>
-  </si>
-  <si>
-    <t>美しき幻獣</t>
-  </si>
-  <si>
-    <t>遺群嶺の火竜</t>
-  </si>
-  <si>
-    <t>リオレウスの翼破壊</t>
-  </si>
-  <si>
-    <t>海竜、沈降開始</t>
-  </si>
-  <si>
-    <t>ラギアクルス１頭の狩猟</t>
-  </si>
-  <si>
-    <t>雪山、雪玉、雪合戦！！</t>
-  </si>
-  <si>
-    <t>ドドブランゴ１頭とウルクスス１頭の狩猟</t>
   </si>
   <si>
     <t>旧砂漠でゆらめく蜃気楼</t>
@@ -3841,8 +3946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J368"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B272" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="G281" sqref="G281"/>
+    <sheetView tabSelected="1" topLeftCell="F313" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="G324" sqref="G324"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12623,17 +12728,20 @@
       <c r="A283" t="s">
         <v>550</v>
       </c>
+      <c r="B283" t="s">
+        <v>551</v>
+      </c>
       <c r="C283" t="s">
         <v>967</v>
       </c>
       <c r="D283" t="s">
-        <v>205</v>
+        <v>535</v>
       </c>
       <c r="E283" t="s">
         <v>14</v>
       </c>
       <c r="F283" t="s">
-        <v>968</v>
+        <v>305</v>
       </c>
       <c r="G283" t="s">
         <v>27</v>
@@ -12650,22 +12758,25 @@
     </row>
     <row r="284" spans="1:10">
       <c r="A284" t="s">
+        <v>968</v>
+      </c>
+      <c r="B284" t="s">
         <v>969</v>
       </c>
       <c r="C284" t="s">
         <v>967</v>
       </c>
       <c r="D284" t="s">
-        <v>79</v>
+        <v>970</v>
       </c>
       <c r="E284" t="s">
         <v>14</v>
       </c>
       <c r="F284" t="s">
-        <v>970</v>
+        <v>934</v>
       </c>
       <c r="G284" t="s">
-        <v>971</v>
+        <v>619</v>
       </c>
       <c r="H284" t="s">
         <v>181</v>
@@ -12679,19 +12790,22 @@
     </row>
     <row r="285" spans="1:10">
       <c r="A285" t="s">
+        <v>971</v>
+      </c>
+      <c r="B285" t="s">
         <v>972</v>
       </c>
       <c r="C285" t="s">
         <v>967</v>
       </c>
       <c r="D285" t="s">
-        <v>86</v>
+        <v>973</v>
       </c>
       <c r="E285" t="s">
         <v>14</v>
       </c>
       <c r="F285" t="s">
-        <v>968</v>
+        <v>305</v>
       </c>
       <c r="G285" t="s">
         <v>27</v>
@@ -12708,19 +12822,22 @@
     </row>
     <row r="286" spans="1:10">
       <c r="A286" t="s">
-        <v>973</v>
+        <v>974</v>
+      </c>
+      <c r="B286" t="s">
+        <v>975</v>
       </c>
       <c r="C286" t="s">
         <v>967</v>
       </c>
       <c r="D286" t="s">
-        <v>205</v>
+        <v>535</v>
       </c>
       <c r="E286" t="s">
         <v>14</v>
       </c>
       <c r="F286" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="G286" t="s">
         <v>27</v>
@@ -12737,22 +12854,25 @@
     </row>
     <row r="287" spans="1:10">
       <c r="A287" t="s">
-        <v>975</v>
+        <v>977</v>
+      </c>
+      <c r="B287" t="s">
+        <v>978</v>
       </c>
       <c r="C287" t="s">
         <v>967</v>
       </c>
       <c r="D287" t="s">
-        <v>171</v>
+        <v>13</v>
       </c>
       <c r="E287" t="s">
         <v>14</v>
       </c>
       <c r="F287" t="s">
-        <v>976</v>
+        <v>979</v>
       </c>
       <c r="G287" t="s">
-        <v>977</v>
+        <v>980</v>
       </c>
       <c r="H287" t="s">
         <v>18</v>
@@ -12766,19 +12886,22 @@
     </row>
     <row r="288" spans="1:10">
       <c r="A288" t="s">
-        <v>978</v>
+        <v>981</v>
+      </c>
+      <c r="B288" t="s">
+        <v>982</v>
       </c>
       <c r="C288" t="s">
         <v>967</v>
       </c>
       <c r="D288" t="s">
-        <v>66</v>
+        <v>879</v>
       </c>
       <c r="E288" t="s">
         <v>14</v>
       </c>
       <c r="F288" t="s">
-        <v>167</v>
+        <v>983</v>
       </c>
       <c r="G288" t="s">
         <v>27</v>
@@ -12795,22 +12918,25 @@
     </row>
     <row r="289" spans="1:10">
       <c r="A289" t="s">
-        <v>979</v>
+        <v>984</v>
+      </c>
+      <c r="B289" t="s">
+        <v>985</v>
       </c>
       <c r="C289" t="s">
         <v>967</v>
       </c>
       <c r="D289" t="s">
-        <v>53</v>
+        <v>286</v>
       </c>
       <c r="E289" t="s">
         <v>14</v>
       </c>
       <c r="F289" t="s">
-        <v>980</v>
+        <v>627</v>
       </c>
       <c r="G289" t="s">
-        <v>981</v>
+        <v>986</v>
       </c>
       <c r="H289" t="s">
         <v>18</v>
@@ -12824,28 +12950,31 @@
     </row>
     <row r="290" spans="1:10">
       <c r="A290" t="s">
-        <v>982</v>
+        <v>987</v>
+      </c>
+      <c r="B290" t="s">
+        <v>988</v>
       </c>
       <c r="C290" t="s">
         <v>967</v>
       </c>
       <c r="D290" t="s">
-        <v>184</v>
+        <v>267</v>
       </c>
       <c r="E290" t="s">
         <v>14</v>
       </c>
       <c r="F290" t="s">
-        <v>983</v>
+        <v>989</v>
       </c>
       <c r="G290" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="H290" t="s">
         <v>750</v>
       </c>
       <c r="I290" t="s">
-        <v>985</v>
+        <v>991</v>
       </c>
       <c r="J290" t="s">
         <v>82</v>
@@ -12853,22 +12982,25 @@
     </row>
     <row r="291" spans="1:10">
       <c r="A291" t="s">
-        <v>986</v>
+        <v>992</v>
+      </c>
+      <c r="B291" t="s">
+        <v>993</v>
       </c>
       <c r="C291" t="s">
         <v>967</v>
       </c>
       <c r="D291" t="s">
-        <v>79</v>
+        <v>970</v>
       </c>
       <c r="E291" t="s">
         <v>14</v>
       </c>
       <c r="F291" t="s">
-        <v>987</v>
+        <v>694</v>
       </c>
       <c r="G291" t="s">
-        <v>988</v>
+        <v>994</v>
       </c>
       <c r="H291" t="s">
         <v>23</v>
@@ -12882,19 +13014,22 @@
     </row>
     <row r="292" spans="1:10">
       <c r="A292" t="s">
-        <v>989</v>
+        <v>995</v>
+      </c>
+      <c r="B292" t="s">
+        <v>996</v>
       </c>
       <c r="C292" t="s">
         <v>967</v>
       </c>
       <c r="D292" t="s">
-        <v>112</v>
+        <v>278</v>
       </c>
       <c r="E292" t="s">
         <v>14</v>
       </c>
       <c r="F292" t="s">
-        <v>990</v>
+        <v>997</v>
       </c>
       <c r="G292" t="s">
         <v>27</v>
@@ -12911,19 +13046,22 @@
     </row>
     <row r="293" spans="1:10">
       <c r="A293" t="s">
-        <v>991</v>
+        <v>998</v>
+      </c>
+      <c r="B293" t="s">
+        <v>999</v>
       </c>
       <c r="C293" t="s">
         <v>967</v>
       </c>
       <c r="D293" t="s">
-        <v>79</v>
+        <v>970</v>
       </c>
       <c r="E293" t="s">
         <v>14</v>
       </c>
       <c r="F293" t="s">
-        <v>992</v>
+        <v>1000</v>
       </c>
       <c r="G293" t="s">
         <v>27</v>
@@ -12942,17 +13080,20 @@
       <c r="A294" t="s">
         <v>461</v>
       </c>
+      <c r="B294" t="s">
+        <v>462</v>
+      </c>
       <c r="C294" t="s">
         <v>967</v>
       </c>
       <c r="D294" t="s">
-        <v>158</v>
+        <v>413</v>
       </c>
       <c r="E294" t="s">
         <v>14</v>
       </c>
       <c r="F294" t="s">
-        <v>968</v>
+        <v>305</v>
       </c>
       <c r="G294" t="s">
         <v>27</v>
@@ -12969,19 +13110,22 @@
     </row>
     <row r="295" spans="1:10">
       <c r="A295" t="s">
-        <v>993</v>
+        <v>1001</v>
+      </c>
+      <c r="B295" t="s">
+        <v>1002</v>
       </c>
       <c r="C295" t="s">
         <v>967</v>
       </c>
       <c r="D295" t="s">
-        <v>79</v>
+        <v>970</v>
       </c>
       <c r="E295" t="s">
         <v>14</v>
       </c>
       <c r="F295" t="s">
-        <v>968</v>
+        <v>305</v>
       </c>
       <c r="G295" t="s">
         <v>27</v>
@@ -12998,22 +13142,25 @@
     </row>
     <row r="296" spans="1:10">
       <c r="A296" t="s">
-        <v>994</v>
+        <v>1003</v>
+      </c>
+      <c r="B296" t="s">
+        <v>1004</v>
       </c>
       <c r="C296" t="s">
         <v>967</v>
       </c>
       <c r="D296" t="s">
-        <v>205</v>
+        <v>535</v>
       </c>
       <c r="E296" t="s">
         <v>14</v>
       </c>
       <c r="F296" t="s">
-        <v>995</v>
+        <v>1005</v>
       </c>
       <c r="G296" t="s">
-        <v>47</v>
+        <v>914</v>
       </c>
       <c r="H296" t="s">
         <v>733</v>
@@ -13029,17 +13176,20 @@
       <c r="A297" t="s">
         <v>406</v>
       </c>
+      <c r="B297" t="s">
+        <v>407</v>
+      </c>
       <c r="C297" t="s">
         <v>967</v>
       </c>
       <c r="D297" t="s">
-        <v>248</v>
+        <v>389</v>
       </c>
       <c r="E297" t="s">
         <v>14</v>
       </c>
       <c r="F297" t="s">
-        <v>968</v>
+        <v>305</v>
       </c>
       <c r="G297" t="s">
         <v>27</v>
@@ -13056,22 +13206,25 @@
     </row>
     <row r="298" spans="1:10">
       <c r="A298" t="s">
-        <v>996</v>
+        <v>1006</v>
+      </c>
+      <c r="B298" t="s">
+        <v>1007</v>
       </c>
       <c r="C298" t="s">
         <v>967</v>
       </c>
       <c r="D298" t="s">
-        <v>91</v>
+        <v>872</v>
       </c>
       <c r="E298" t="s">
         <v>14</v>
       </c>
       <c r="F298" t="s">
-        <v>997</v>
+        <v>592</v>
       </c>
       <c r="G298" t="s">
-        <v>998</v>
+        <v>1008</v>
       </c>
       <c r="H298" t="s">
         <v>562</v>
@@ -13085,22 +13238,25 @@
     </row>
     <row r="299" spans="1:10">
       <c r="A299" t="s">
-        <v>999</v>
+        <v>1009</v>
+      </c>
+      <c r="B299" t="s">
+        <v>1010</v>
       </c>
       <c r="C299" t="s">
         <v>967</v>
       </c>
       <c r="D299" t="s">
-        <v>205</v>
+        <v>535</v>
       </c>
       <c r="E299" t="s">
         <v>14</v>
       </c>
       <c r="F299" t="s">
-        <v>1000</v>
+        <v>710</v>
       </c>
       <c r="G299" t="s">
-        <v>1001</v>
+        <v>1011</v>
       </c>
       <c r="H299" t="s">
         <v>733</v>
@@ -13114,22 +13270,25 @@
     </row>
     <row r="300" spans="1:10">
       <c r="A300" t="s">
-        <v>1002</v>
+        <v>1012</v>
+      </c>
+      <c r="B300" t="s">
+        <v>1013</v>
       </c>
       <c r="C300" t="s">
         <v>967</v>
       </c>
       <c r="D300" t="s">
-        <v>122</v>
+        <v>1014</v>
       </c>
       <c r="E300" t="s">
         <v>14</v>
       </c>
       <c r="F300" t="s">
-        <v>1000</v>
+        <v>710</v>
       </c>
       <c r="G300" t="s">
-        <v>109</v>
+        <v>288</v>
       </c>
       <c r="H300" t="s">
         <v>733</v>
@@ -13143,22 +13302,25 @@
     </row>
     <row r="301" spans="1:10">
       <c r="A301" t="s">
-        <v>1003</v>
+        <v>1015</v>
+      </c>
+      <c r="B301" t="s">
+        <v>1016</v>
       </c>
       <c r="C301" t="s">
         <v>967</v>
       </c>
       <c r="D301" t="s">
-        <v>248</v>
+        <v>389</v>
       </c>
       <c r="E301" t="s">
         <v>14</v>
       </c>
       <c r="F301" t="s">
-        <v>1004</v>
+        <v>1017</v>
       </c>
       <c r="G301" t="s">
-        <v>109</v>
+        <v>288</v>
       </c>
       <c r="H301" t="s">
         <v>562</v>
@@ -13172,22 +13334,25 @@
     </row>
     <row r="302" spans="1:10">
       <c r="A302" t="s">
-        <v>1005</v>
+        <v>1018</v>
+      </c>
+      <c r="B302" t="s">
+        <v>1019</v>
       </c>
       <c r="C302" t="s">
         <v>967</v>
       </c>
       <c r="D302" t="s">
-        <v>45</v>
+        <v>941</v>
       </c>
       <c r="E302" t="s">
         <v>14</v>
       </c>
       <c r="F302" t="s">
-        <v>1006</v>
+        <v>1020</v>
       </c>
       <c r="G302" t="s">
-        <v>1007</v>
+        <v>369</v>
       </c>
       <c r="H302" t="s">
         <v>562</v>
@@ -13201,22 +13366,25 @@
     </row>
     <row r="303" spans="1:10">
       <c r="A303" t="s">
-        <v>1008</v>
+        <v>1021</v>
+      </c>
+      <c r="B303" t="s">
+        <v>1022</v>
       </c>
       <c r="C303" t="s">
         <v>967</v>
       </c>
       <c r="D303" t="s">
-        <v>195</v>
+        <v>309</v>
       </c>
       <c r="E303" t="s">
         <v>14</v>
       </c>
       <c r="F303" t="s">
-        <v>1009</v>
+        <v>1023</v>
       </c>
       <c r="G303" t="s">
-        <v>47</v>
+        <v>914</v>
       </c>
       <c r="H303" t="s">
         <v>23</v>
@@ -13230,22 +13398,25 @@
     </row>
     <row r="304" spans="1:10">
       <c r="A304" t="s">
-        <v>1010</v>
+        <v>1024</v>
+      </c>
+      <c r="B304" t="s">
+        <v>1025</v>
       </c>
       <c r="C304" t="s">
         <v>967</v>
       </c>
       <c r="D304" t="s">
-        <v>248</v>
+        <v>389</v>
       </c>
       <c r="E304" t="s">
         <v>14</v>
       </c>
       <c r="F304" t="s">
-        <v>1011</v>
+        <v>1026</v>
       </c>
       <c r="G304" t="s">
-        <v>1007</v>
+        <v>369</v>
       </c>
       <c r="H304" t="s">
         <v>69</v>
@@ -13259,28 +13430,31 @@
     </row>
     <row r="305" spans="1:10">
       <c r="A305" t="s">
-        <v>1012</v>
+        <v>1027</v>
+      </c>
+      <c r="B305" t="s">
+        <v>1028</v>
       </c>
       <c r="C305" t="s">
         <v>967</v>
       </c>
       <c r="D305" t="s">
-        <v>158</v>
+        <v>413</v>
       </c>
       <c r="E305" t="s">
         <v>14</v>
       </c>
       <c r="F305" t="s">
-        <v>1013</v>
+        <v>1029</v>
       </c>
       <c r="G305" t="s">
-        <v>47</v>
+        <v>914</v>
       </c>
       <c r="H305" t="s">
         <v>750</v>
       </c>
       <c r="I305" t="s">
-        <v>985</v>
+        <v>991</v>
       </c>
       <c r="J305" t="s">
         <v>50</v>
@@ -13288,22 +13462,25 @@
     </row>
     <row r="306" spans="1:10">
       <c r="A306" t="s">
-        <v>1014</v>
+        <v>1030</v>
+      </c>
+      <c r="B306" t="s">
+        <v>1031</v>
       </c>
       <c r="C306" t="s">
         <v>967</v>
       </c>
       <c r="D306" t="s">
-        <v>66</v>
+        <v>879</v>
       </c>
       <c r="E306" t="s">
         <v>14</v>
       </c>
       <c r="F306" t="s">
-        <v>1015</v>
+        <v>513</v>
       </c>
       <c r="G306" t="s">
-        <v>1016</v>
+        <v>1032</v>
       </c>
       <c r="H306" t="s">
         <v>181</v>
@@ -13317,22 +13494,25 @@
     </row>
     <row r="307" spans="1:10">
       <c r="A307" t="s">
-        <v>1017</v>
+        <v>1033</v>
+      </c>
+      <c r="B307" t="s">
+        <v>1034</v>
       </c>
       <c r="C307" t="s">
         <v>967</v>
       </c>
       <c r="D307" t="s">
-        <v>86</v>
+        <v>973</v>
       </c>
       <c r="E307" t="s">
         <v>14</v>
       </c>
       <c r="F307" t="s">
-        <v>1018</v>
+        <v>1035</v>
       </c>
       <c r="G307" t="s">
-        <v>1019</v>
+        <v>1036</v>
       </c>
       <c r="H307" t="s">
         <v>181</v>
@@ -13346,22 +13526,25 @@
     </row>
     <row r="308" spans="1:10">
       <c r="A308" t="s">
-        <v>1020</v>
+        <v>1037</v>
+      </c>
+      <c r="B308" t="s">
+        <v>1038</v>
       </c>
       <c r="C308" t="s">
         <v>967</v>
       </c>
       <c r="D308" t="s">
-        <v>91</v>
+        <v>872</v>
       </c>
       <c r="E308" t="s">
         <v>14</v>
       </c>
       <c r="F308" t="s">
-        <v>971</v>
+        <v>619</v>
       </c>
       <c r="G308" t="s">
-        <v>1021</v>
+        <v>603</v>
       </c>
       <c r="H308" t="s">
         <v>23</v>
@@ -13375,22 +13558,25 @@
     </row>
     <row r="309" spans="1:10">
       <c r="A309" t="s">
-        <v>1022</v>
+        <v>1039</v>
+      </c>
+      <c r="B309" t="s">
+        <v>1040</v>
       </c>
       <c r="C309" t="s">
         <v>967</v>
       </c>
       <c r="D309" t="s">
-        <v>66</v>
+        <v>879</v>
       </c>
       <c r="E309" t="s">
         <v>14</v>
       </c>
       <c r="F309" t="s">
-        <v>1023</v>
+        <v>575</v>
       </c>
       <c r="G309" t="s">
-        <v>1024</v>
+        <v>1041</v>
       </c>
       <c r="H309" t="s">
         <v>181</v>
@@ -13404,19 +13590,22 @@
     </row>
     <row r="310" spans="1:10">
       <c r="A310" t="s">
-        <v>1025</v>
+        <v>1042</v>
+      </c>
+      <c r="B310" t="s">
+        <v>1043</v>
       </c>
       <c r="C310" t="s">
         <v>967</v>
       </c>
       <c r="D310" t="s">
-        <v>143</v>
+        <v>850</v>
       </c>
       <c r="E310" t="s">
         <v>14</v>
       </c>
       <c r="F310" t="s">
-        <v>1026</v>
+        <v>1044</v>
       </c>
       <c r="G310" t="s">
         <v>27</v>
@@ -13433,22 +13622,25 @@
     </row>
     <row r="311" spans="1:10">
       <c r="A311" t="s">
-        <v>1027</v>
+        <v>1045</v>
+      </c>
+      <c r="B311" t="s">
+        <v>1046</v>
       </c>
       <c r="C311" t="s">
         <v>967</v>
       </c>
       <c r="D311" t="s">
-        <v>91</v>
+        <v>872</v>
       </c>
       <c r="E311" t="s">
         <v>14</v>
       </c>
       <c r="F311" t="s">
-        <v>1028</v>
+        <v>1047</v>
       </c>
       <c r="G311" t="s">
-        <v>1004</v>
+        <v>1017</v>
       </c>
       <c r="H311" t="s">
         <v>18</v>
@@ -13462,22 +13654,25 @@
     </row>
     <row r="312" spans="1:10">
       <c r="A312" t="s">
-        <v>1029</v>
+        <v>1048</v>
+      </c>
+      <c r="B312" t="s">
+        <v>1049</v>
       </c>
       <c r="C312" t="s">
         <v>967</v>
       </c>
       <c r="D312" t="s">
-        <v>79</v>
+        <v>970</v>
       </c>
       <c r="E312" t="s">
         <v>14</v>
       </c>
       <c r="F312" t="s">
-        <v>1030</v>
+        <v>1050</v>
       </c>
       <c r="G312" t="s">
-        <v>1031</v>
+        <v>1051</v>
       </c>
       <c r="H312" t="s">
         <v>18</v>
@@ -13491,19 +13686,22 @@
     </row>
     <row r="313" spans="1:10">
       <c r="A313" t="s">
-        <v>1032</v>
+        <v>1052</v>
+      </c>
+      <c r="B313" t="s">
+        <v>1053</v>
       </c>
       <c r="C313" t="s">
         <v>967</v>
       </c>
       <c r="D313" t="s">
-        <v>91</v>
+        <v>872</v>
       </c>
       <c r="E313" t="s">
         <v>14</v>
       </c>
       <c r="F313" t="s">
-        <v>981</v>
+        <v>986</v>
       </c>
       <c r="G313" t="s">
         <v>27</v>
@@ -13520,22 +13718,25 @@
     </row>
     <row r="314" spans="1:10">
       <c r="A314" t="s">
-        <v>1033</v>
+        <v>1054</v>
+      </c>
+      <c r="B314" t="s">
+        <v>1055</v>
       </c>
       <c r="C314" t="s">
         <v>967</v>
       </c>
       <c r="D314" t="s">
-        <v>112</v>
+        <v>278</v>
       </c>
       <c r="E314" t="s">
         <v>14</v>
       </c>
       <c r="F314" t="s">
-        <v>1034</v>
+        <v>554</v>
       </c>
       <c r="G314" t="s">
-        <v>1035</v>
+        <v>1056</v>
       </c>
       <c r="H314" t="s">
         <v>23</v>
@@ -13549,19 +13750,22 @@
     </row>
     <row r="315" spans="1:10">
       <c r="A315" t="s">
-        <v>1036</v>
+        <v>1057</v>
+      </c>
+      <c r="B315" t="s">
+        <v>1058</v>
       </c>
       <c r="C315" t="s">
         <v>967</v>
       </c>
       <c r="D315" t="s">
-        <v>91</v>
+        <v>872</v>
       </c>
       <c r="E315" t="s">
         <v>14</v>
       </c>
       <c r="F315" t="s">
-        <v>1037</v>
+        <v>1059</v>
       </c>
       <c r="G315" t="s">
         <v>27</v>
@@ -13578,22 +13782,25 @@
     </row>
     <row r="316" spans="1:10">
       <c r="A316" t="s">
-        <v>1038</v>
+        <v>1060</v>
+      </c>
+      <c r="B316" t="s">
+        <v>1061</v>
       </c>
       <c r="C316" t="s">
         <v>967</v>
       </c>
       <c r="D316" t="s">
-        <v>91</v>
+        <v>872</v>
       </c>
       <c r="E316" t="s">
         <v>14</v>
       </c>
       <c r="F316" t="s">
-        <v>1039</v>
+        <v>538</v>
       </c>
       <c r="G316" t="s">
-        <v>1040</v>
+        <v>624</v>
       </c>
       <c r="H316" t="s">
         <v>23</v>
@@ -13607,19 +13814,22 @@
     </row>
     <row r="317" spans="1:10">
       <c r="A317" t="s">
-        <v>1041</v>
+        <v>1062</v>
+      </c>
+      <c r="B317" t="s">
+        <v>1063</v>
       </c>
       <c r="C317" t="s">
         <v>967</v>
       </c>
       <c r="D317" t="s">
-        <v>122</v>
+        <v>1014</v>
       </c>
       <c r="E317" t="s">
         <v>14</v>
       </c>
       <c r="F317" t="s">
-        <v>968</v>
+        <v>305</v>
       </c>
       <c r="G317" t="s">
         <v>27</v>
@@ -13636,22 +13846,25 @@
     </row>
     <row r="318" spans="1:10">
       <c r="A318" t="s">
-        <v>1042</v>
+        <v>1064</v>
+      </c>
+      <c r="B318" t="s">
+        <v>1065</v>
       </c>
       <c r="C318" t="s">
         <v>967</v>
       </c>
       <c r="D318" t="s">
-        <v>158</v>
+        <v>413</v>
       </c>
       <c r="E318" t="s">
         <v>14</v>
       </c>
       <c r="F318" t="s">
-        <v>992</v>
+        <v>1000</v>
       </c>
       <c r="G318" t="s">
-        <v>1043</v>
+        <v>1066</v>
       </c>
       <c r="H318" t="s">
         <v>23</v>
@@ -13665,22 +13878,25 @@
     </row>
     <row r="319" spans="1:10">
       <c r="A319" t="s">
-        <v>1044</v>
+        <v>1067</v>
+      </c>
+      <c r="B319" t="s">
+        <v>1068</v>
       </c>
       <c r="C319" t="s">
         <v>967</v>
       </c>
       <c r="D319" t="s">
-        <v>86</v>
+        <v>973</v>
       </c>
       <c r="E319" t="s">
         <v>14</v>
       </c>
       <c r="F319" t="s">
-        <v>1045</v>
+        <v>1069</v>
       </c>
       <c r="G319" t="s">
-        <v>1046</v>
+        <v>1070</v>
       </c>
       <c r="H319" t="s">
         <v>562</v>
@@ -13694,22 +13910,25 @@
     </row>
     <row r="320" spans="1:10">
       <c r="A320" t="s">
-        <v>1047</v>
+        <v>1071</v>
+      </c>
+      <c r="B320" t="s">
+        <v>1072</v>
       </c>
       <c r="C320" t="s">
         <v>967</v>
       </c>
       <c r="D320" t="s">
-        <v>79</v>
+        <v>970</v>
       </c>
       <c r="E320" t="s">
         <v>14</v>
       </c>
       <c r="F320" t="s">
-        <v>1048</v>
+        <v>1073</v>
       </c>
       <c r="G320" t="s">
-        <v>992</v>
+        <v>1000</v>
       </c>
       <c r="H320" t="s">
         <v>18</v>
@@ -13723,22 +13942,25 @@
     </row>
     <row r="321" spans="1:10">
       <c r="A321" t="s">
-        <v>1049</v>
+        <v>1074</v>
+      </c>
+      <c r="B321" t="s">
+        <v>1075</v>
       </c>
       <c r="C321" t="s">
         <v>967</v>
       </c>
       <c r="D321" t="s">
-        <v>112</v>
+        <v>278</v>
       </c>
       <c r="E321" t="s">
         <v>14</v>
       </c>
       <c r="F321" t="s">
-        <v>1018</v>
+        <v>1035</v>
       </c>
       <c r="G321" t="s">
-        <v>1050</v>
+        <v>1076</v>
       </c>
       <c r="H321" t="s">
         <v>181</v>
@@ -13752,19 +13974,22 @@
     </row>
     <row r="322" spans="1:10">
       <c r="A322" t="s">
-        <v>1051</v>
+        <v>1077</v>
+      </c>
+      <c r="B322" t="s">
+        <v>1078</v>
       </c>
       <c r="C322" t="s">
         <v>967</v>
       </c>
       <c r="D322" t="s">
-        <v>143</v>
+        <v>850</v>
       </c>
       <c r="E322" t="s">
         <v>14</v>
       </c>
       <c r="F322" t="s">
-        <v>1052</v>
+        <v>904</v>
       </c>
       <c r="G322" t="s">
         <v>27</v>
@@ -13781,22 +14006,25 @@
     </row>
     <row r="323" spans="1:10">
       <c r="A323" t="s">
-        <v>1053</v>
+        <v>1079</v>
+      </c>
+      <c r="B323" t="s">
+        <v>1080</v>
       </c>
       <c r="C323" t="s">
         <v>967</v>
       </c>
       <c r="D323" t="s">
-        <v>143</v>
+        <v>850</v>
       </c>
       <c r="E323" t="s">
         <v>14</v>
       </c>
       <c r="F323" t="s">
-        <v>1054</v>
+        <v>1081</v>
       </c>
       <c r="G323" t="s">
-        <v>109</v>
+        <v>288</v>
       </c>
       <c r="H323" t="s">
         <v>69</v>
@@ -13810,22 +14038,25 @@
     </row>
     <row r="324" spans="1:10">
       <c r="A324" t="s">
-        <v>1055</v>
+        <v>1082</v>
+      </c>
+      <c r="B324" t="s">
+        <v>1083</v>
       </c>
       <c r="C324" t="s">
         <v>967</v>
       </c>
       <c r="D324" t="s">
-        <v>158</v>
+        <v>413</v>
       </c>
       <c r="E324" t="s">
         <v>14</v>
       </c>
       <c r="F324" t="s">
-        <v>1056</v>
+        <v>1084</v>
       </c>
       <c r="G324" t="s">
-        <v>1007</v>
+        <v>369</v>
       </c>
       <c r="H324" t="s">
         <v>750</v>
@@ -13839,13 +14070,16 @@
     </row>
     <row r="325" spans="1:10">
       <c r="A325" t="s">
-        <v>1057</v>
+        <v>1085</v>
+      </c>
+      <c r="B325" t="s">
+        <v>1086</v>
       </c>
       <c r="C325" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D325" t="s">
-        <v>66</v>
+        <v>879</v>
       </c>
       <c r="E325" t="s">
         <v>14</v>
@@ -13854,7 +14088,7 @@
         <v>113</v>
       </c>
       <c r="G325" t="s">
-        <v>1059</v>
+        <v>1088</v>
       </c>
       <c r="H325" t="s">
         <v>69</v>
@@ -13868,19 +14102,22 @@
     </row>
     <row r="326" spans="1:10">
       <c r="A326" t="s">
-        <v>1060</v>
+        <v>1089</v>
+      </c>
+      <c r="B326" t="s">
+        <v>1090</v>
       </c>
       <c r="C326" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D326" t="s">
-        <v>184</v>
+        <v>267</v>
       </c>
       <c r="E326" t="s">
         <v>14</v>
       </c>
       <c r="F326" t="s">
-        <v>1061</v>
+        <v>1091</v>
       </c>
       <c r="G326" t="s">
         <v>27</v>
@@ -13897,19 +14134,22 @@
     </row>
     <row r="327" spans="1:10">
       <c r="A327" t="s">
-        <v>1062</v>
+        <v>1092</v>
+      </c>
+      <c r="B327" t="s">
+        <v>1093</v>
       </c>
       <c r="C327" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D327" t="s">
-        <v>86</v>
+        <v>973</v>
       </c>
       <c r="E327" t="s">
         <v>14</v>
       </c>
       <c r="F327" t="s">
-        <v>1063</v>
+        <v>1094</v>
       </c>
       <c r="G327" t="s">
         <v>27</v>
@@ -13926,10 +14166,13 @@
     </row>
     <row r="328" spans="1:10">
       <c r="A328" t="s">
-        <v>1064</v>
+        <v>1095</v>
+      </c>
+      <c r="B328" t="s">
+        <v>1096</v>
       </c>
       <c r="C328" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D328" t="s">
         <v>53</v>
@@ -13938,7 +14181,7 @@
         <v>14</v>
       </c>
       <c r="F328" t="s">
-        <v>1065</v>
+        <v>1097</v>
       </c>
       <c r="G328" t="s">
         <v>27</v>
@@ -13955,10 +14198,13 @@
     </row>
     <row r="329" spans="1:10">
       <c r="A329" t="s">
-        <v>1066</v>
+        <v>1098</v>
+      </c>
+      <c r="B329" t="s">
+        <v>1099</v>
       </c>
       <c r="C329" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D329" t="s">
         <v>171</v>
@@ -13967,7 +14213,7 @@
         <v>14</v>
       </c>
       <c r="F329" t="s">
-        <v>1067</v>
+        <v>1100</v>
       </c>
       <c r="G329" t="s">
         <v>27</v>
@@ -13981,10 +14227,10 @@
     </row>
     <row r="330" spans="1:10">
       <c r="A330" t="s">
-        <v>1068</v>
+        <v>1101</v>
       </c>
       <c r="C330" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D330" t="s">
         <v>86</v>
@@ -13993,16 +14239,16 @@
         <v>14</v>
       </c>
       <c r="F330" t="s">
-        <v>1069</v>
+        <v>1102</v>
       </c>
       <c r="G330" t="s">
-        <v>1070</v>
+        <v>1103</v>
       </c>
       <c r="H330" t="s">
         <v>229</v>
       </c>
       <c r="I330" t="s">
-        <v>1071</v>
+        <v>1104</v>
       </c>
       <c r="J330" t="s">
         <v>450</v>
@@ -14010,10 +14256,10 @@
     </row>
     <row r="331" spans="1:10">
       <c r="A331" t="s">
-        <v>1072</v>
+        <v>1105</v>
       </c>
       <c r="C331" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D331" t="s">
         <v>91</v>
@@ -14022,10 +14268,10 @@
         <v>14</v>
       </c>
       <c r="F331" t="s">
-        <v>1073</v>
+        <v>1106</v>
       </c>
       <c r="G331" t="s">
-        <v>1074</v>
+        <v>1107</v>
       </c>
       <c r="H331" t="s">
         <v>48</v>
@@ -14039,10 +14285,10 @@
     </row>
     <row r="332" spans="1:10">
       <c r="A332" t="s">
-        <v>1075</v>
+        <v>1108</v>
       </c>
       <c r="C332" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D332" t="s">
         <v>79</v>
@@ -14054,7 +14300,7 @@
         <v>259</v>
       </c>
       <c r="G332" t="s">
-        <v>1076</v>
+        <v>1109</v>
       </c>
       <c r="H332" t="s">
         <v>750</v>
@@ -14068,10 +14314,10 @@
     </row>
     <row r="333" spans="1:10">
       <c r="A333" t="s">
-        <v>1077</v>
+        <v>1110</v>
       </c>
       <c r="C333" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D333" t="s">
         <v>79</v>
@@ -14080,10 +14326,10 @@
         <v>14</v>
       </c>
       <c r="F333" t="s">
-        <v>1078</v>
+        <v>1111</v>
       </c>
       <c r="G333" t="s">
-        <v>1079</v>
+        <v>1112</v>
       </c>
       <c r="H333" t="s">
         <v>733</v>
@@ -14097,10 +14343,10 @@
     </row>
     <row r="334" spans="1:10">
       <c r="A334" t="s">
-        <v>1080</v>
+        <v>1113</v>
       </c>
       <c r="C334" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D334" t="s">
         <v>86</v>
@@ -14126,10 +14372,10 @@
     </row>
     <row r="335" spans="1:10">
       <c r="A335" t="s">
-        <v>1081</v>
+        <v>1114</v>
       </c>
       <c r="C335" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D335" t="s">
         <v>184</v>
@@ -14138,7 +14384,7 @@
         <v>14</v>
       </c>
       <c r="F335" t="s">
-        <v>970</v>
+        <v>1115</v>
       </c>
       <c r="G335" t="s">
         <v>251</v>
@@ -14155,10 +14401,10 @@
     </row>
     <row r="336" spans="1:10">
       <c r="A336" t="s">
-        <v>1082</v>
+        <v>1116</v>
       </c>
       <c r="C336" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D336" t="s">
         <v>195</v>
@@ -14167,7 +14413,7 @@
         <v>14</v>
       </c>
       <c r="F336" t="s">
-        <v>1083</v>
+        <v>1117</v>
       </c>
       <c r="G336" t="s">
         <v>109</v>
@@ -14176,7 +14422,7 @@
         <v>48</v>
       </c>
       <c r="I336" t="s">
-        <v>1084</v>
+        <v>1118</v>
       </c>
       <c r="J336" t="s">
         <v>450</v>
@@ -14184,10 +14430,10 @@
     </row>
     <row r="337" spans="1:10">
       <c r="A337" t="s">
-        <v>1085</v>
+        <v>1119</v>
       </c>
       <c r="C337" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D337" t="s">
         <v>122</v>
@@ -14196,10 +14442,10 @@
         <v>14</v>
       </c>
       <c r="F337" t="s">
-        <v>1086</v>
+        <v>1120</v>
       </c>
       <c r="G337" t="s">
-        <v>1087</v>
+        <v>1121</v>
       </c>
       <c r="H337" t="s">
         <v>48</v>
@@ -14213,10 +14459,10 @@
     </row>
     <row r="338" spans="1:10">
       <c r="A338" t="s">
-        <v>1088</v>
+        <v>1122</v>
       </c>
       <c r="C338" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D338" t="s">
         <v>205</v>
@@ -14242,10 +14488,10 @@
     </row>
     <row r="339" spans="1:10">
       <c r="A339" t="s">
-        <v>1089</v>
+        <v>1123</v>
       </c>
       <c r="C339" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D339" t="s">
         <v>171</v>
@@ -14263,7 +14509,7 @@
         <v>241</v>
       </c>
       <c r="I339" t="s">
-        <v>1090</v>
+        <v>1124</v>
       </c>
       <c r="J339" t="s">
         <v>58</v>
@@ -14271,10 +14517,10 @@
     </row>
     <row r="340" spans="1:10">
       <c r="A340" t="s">
-        <v>1091</v>
+        <v>1125</v>
       </c>
       <c r="C340" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D340" t="s">
         <v>91</v>
@@ -14283,10 +14529,10 @@
         <v>14</v>
       </c>
       <c r="F340" t="s">
-        <v>1092</v>
+        <v>1126</v>
       </c>
       <c r="G340" t="s">
-        <v>1093</v>
+        <v>1127</v>
       </c>
       <c r="H340" t="s">
         <v>750</v>
@@ -14300,10 +14546,10 @@
     </row>
     <row r="341" spans="1:10">
       <c r="A341" t="s">
-        <v>1094</v>
+        <v>1128</v>
       </c>
       <c r="C341" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D341" t="s">
         <v>45</v>
@@ -14315,13 +14561,13 @@
         <v>54</v>
       </c>
       <c r="G341" t="s">
-        <v>1095</v>
+        <v>1129</v>
       </c>
       <c r="H341" t="s">
         <v>229</v>
       </c>
       <c r="I341" t="s">
-        <v>1071</v>
+        <v>1104</v>
       </c>
       <c r="J341" t="s">
         <v>450</v>
@@ -14329,10 +14575,10 @@
     </row>
     <row r="342" spans="1:10">
       <c r="A342" t="s">
-        <v>1096</v>
+        <v>1130</v>
       </c>
       <c r="C342" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D342" t="s">
         <v>91</v>
@@ -14341,7 +14587,7 @@
         <v>14</v>
       </c>
       <c r="F342" t="s">
-        <v>1067</v>
+        <v>1100</v>
       </c>
       <c r="G342" t="s">
         <v>27</v>
@@ -14358,10 +14604,10 @@
     </row>
     <row r="343" spans="1:10">
       <c r="A343" t="s">
-        <v>1097</v>
+        <v>1131</v>
       </c>
       <c r="C343" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D343" t="s">
         <v>91</v>
@@ -14373,7 +14619,7 @@
         <v>251</v>
       </c>
       <c r="G343" t="s">
-        <v>1098</v>
+        <v>1132</v>
       </c>
       <c r="H343" t="s">
         <v>733</v>
@@ -14387,10 +14633,10 @@
     </row>
     <row r="344" spans="1:10">
       <c r="A344" t="s">
-        <v>1099</v>
+        <v>1133</v>
       </c>
       <c r="C344" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D344" t="s">
         <v>79</v>
@@ -14399,7 +14645,7 @@
         <v>14</v>
       </c>
       <c r="F344" t="s">
-        <v>1100</v>
+        <v>1134</v>
       </c>
       <c r="G344" t="s">
         <v>47</v>
@@ -14416,10 +14662,10 @@
     </row>
     <row r="345" spans="1:10">
       <c r="A345" t="s">
-        <v>1101</v>
+        <v>1135</v>
       </c>
       <c r="C345" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D345" t="s">
         <v>112</v>
@@ -14428,10 +14674,10 @@
         <v>14</v>
       </c>
       <c r="F345" t="s">
-        <v>1102</v>
+        <v>1136</v>
       </c>
       <c r="G345" t="s">
-        <v>1007</v>
+        <v>1137</v>
       </c>
       <c r="H345" t="s">
         <v>750</v>
@@ -14445,10 +14691,10 @@
     </row>
     <row r="346" spans="1:10">
       <c r="A346" t="s">
-        <v>1103</v>
+        <v>1138</v>
       </c>
       <c r="C346" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D346" t="s">
         <v>195</v>
@@ -14460,7 +14706,7 @@
         <v>54</v>
       </c>
       <c r="G346" t="s">
-        <v>1095</v>
+        <v>1129</v>
       </c>
       <c r="H346" t="s">
         <v>114</v>
@@ -14474,10 +14720,10 @@
     </row>
     <row r="347" spans="1:10">
       <c r="A347" t="s">
-        <v>1104</v>
+        <v>1139</v>
       </c>
       <c r="C347" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D347" t="s">
         <v>122</v>
@@ -14486,7 +14732,7 @@
         <v>14</v>
       </c>
       <c r="F347" t="s">
-        <v>1105</v>
+        <v>1140</v>
       </c>
       <c r="G347" t="s">
         <v>27</v>
@@ -14503,10 +14749,10 @@
     </row>
     <row r="348" spans="1:10">
       <c r="A348" t="s">
-        <v>1106</v>
+        <v>1141</v>
       </c>
       <c r="C348" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D348" t="s">
         <v>112</v>
@@ -14515,10 +14761,10 @@
         <v>14</v>
       </c>
       <c r="F348" t="s">
-        <v>1107</v>
+        <v>1142</v>
       </c>
       <c r="G348" t="s">
-        <v>1108</v>
+        <v>1143</v>
       </c>
       <c r="H348" t="s">
         <v>241</v>
@@ -14532,10 +14778,10 @@
     </row>
     <row r="349" spans="1:10">
       <c r="A349" t="s">
-        <v>1109</v>
+        <v>1144</v>
       </c>
       <c r="C349" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D349" t="s">
         <v>143</v>
@@ -14544,10 +14790,10 @@
         <v>14</v>
       </c>
       <c r="F349" t="s">
-        <v>1110</v>
+        <v>1145</v>
       </c>
       <c r="G349" t="s">
-        <v>1111</v>
+        <v>1146</v>
       </c>
       <c r="H349" t="s">
         <v>241</v>
@@ -14561,10 +14807,10 @@
     </row>
     <row r="350" spans="1:10">
       <c r="A350" t="s">
-        <v>1112</v>
+        <v>1147</v>
       </c>
       <c r="C350" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D350" t="s">
         <v>45</v>
@@ -14573,10 +14819,10 @@
         <v>14</v>
       </c>
       <c r="F350" t="s">
-        <v>1061</v>
+        <v>1091</v>
       </c>
       <c r="G350" t="s">
-        <v>1113</v>
+        <v>1148</v>
       </c>
       <c r="H350" t="s">
         <v>750</v>
@@ -14590,10 +14836,10 @@
     </row>
     <row r="351" spans="1:10">
       <c r="A351" t="s">
-        <v>1114</v>
+        <v>1149</v>
       </c>
       <c r="C351" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D351" t="s">
         <v>91</v>
@@ -14602,7 +14848,7 @@
         <v>14</v>
       </c>
       <c r="F351" t="s">
-        <v>1115</v>
+        <v>1150</v>
       </c>
       <c r="G351" t="s">
         <v>27</v>
@@ -14619,10 +14865,10 @@
     </row>
     <row r="352" spans="1:10">
       <c r="A352" t="s">
-        <v>1116</v>
+        <v>1151</v>
       </c>
       <c r="C352" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D352" t="s">
         <v>122</v>
@@ -14648,10 +14894,10 @@
     </row>
     <row r="353" spans="1:10">
       <c r="A353" t="s">
-        <v>1117</v>
+        <v>1152</v>
       </c>
       <c r="C353" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D353" t="s">
         <v>112</v>
@@ -14660,7 +14906,7 @@
         <v>14</v>
       </c>
       <c r="F353" t="s">
-        <v>1118</v>
+        <v>1153</v>
       </c>
       <c r="G353" t="s">
         <v>27</v>
@@ -14677,10 +14923,10 @@
     </row>
     <row r="354" spans="1:10">
       <c r="A354" t="s">
-        <v>1119</v>
+        <v>1154</v>
       </c>
       <c r="C354" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D354" t="s">
         <v>86</v>
@@ -14689,10 +14935,10 @@
         <v>14</v>
       </c>
       <c r="F354" t="s">
-        <v>1120</v>
+        <v>1155</v>
       </c>
       <c r="G354" t="s">
-        <v>1121</v>
+        <v>1156</v>
       </c>
       <c r="H354" t="s">
         <v>69</v>
@@ -14706,10 +14952,10 @@
     </row>
     <row r="355" spans="1:10">
       <c r="A355" t="s">
-        <v>1122</v>
+        <v>1157</v>
       </c>
       <c r="C355" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D355" t="s">
         <v>248</v>
@@ -14718,7 +14964,7 @@
         <v>14</v>
       </c>
       <c r="F355" t="s">
-        <v>1123</v>
+        <v>1158</v>
       </c>
       <c r="G355" t="s">
         <v>27</v>
@@ -14735,10 +14981,10 @@
     </row>
     <row r="356" spans="1:10">
       <c r="A356" t="s">
-        <v>1124</v>
+        <v>1159</v>
       </c>
       <c r="C356" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D356" t="s">
         <v>195</v>
@@ -14764,10 +15010,10 @@
     </row>
     <row r="357" spans="1:10">
       <c r="A357" t="s">
-        <v>1125</v>
+        <v>1160</v>
       </c>
       <c r="C357" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D357" t="s">
         <v>79</v>
@@ -14776,7 +15022,7 @@
         <v>14</v>
       </c>
       <c r="F357" t="s">
-        <v>1126</v>
+        <v>1161</v>
       </c>
       <c r="G357" t="s">
         <v>47</v>
@@ -14793,10 +15039,10 @@
     </row>
     <row r="358" spans="1:10">
       <c r="A358" t="s">
-        <v>1127</v>
+        <v>1162</v>
       </c>
       <c r="C358" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D358" t="s">
         <v>79</v>
@@ -14805,10 +15051,10 @@
         <v>14</v>
       </c>
       <c r="F358" t="s">
-        <v>1128</v>
+        <v>1163</v>
       </c>
       <c r="G358" t="s">
-        <v>1129</v>
+        <v>1164</v>
       </c>
       <c r="H358" t="s">
         <v>750</v>
@@ -14825,7 +15071,7 @@
         <v>141</v>
       </c>
       <c r="C359" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D359" t="s">
         <v>143</v>
@@ -14834,10 +15080,10 @@
         <v>14</v>
       </c>
       <c r="F359" t="s">
-        <v>1115</v>
+        <v>1150</v>
       </c>
       <c r="G359" t="s">
-        <v>1130</v>
+        <v>1165</v>
       </c>
       <c r="H359" t="s">
         <v>750</v>
@@ -14851,10 +15097,10 @@
     </row>
     <row r="360" spans="1:10">
       <c r="A360" t="s">
-        <v>1131</v>
+        <v>1166</v>
       </c>
       <c r="C360" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D360" t="s">
         <v>205</v>
@@ -14863,7 +15109,7 @@
         <v>14</v>
       </c>
       <c r="F360" t="s">
-        <v>1132</v>
+        <v>1167</v>
       </c>
       <c r="G360" t="s">
         <v>47</v>
@@ -14872,7 +15118,7 @@
         <v>229</v>
       </c>
       <c r="I360" t="s">
-        <v>1133</v>
+        <v>1168</v>
       </c>
       <c r="J360" t="s">
         <v>50</v>
@@ -14880,10 +15126,10 @@
     </row>
     <row r="361" spans="1:10">
       <c r="A361" t="s">
-        <v>1134</v>
+        <v>1169</v>
       </c>
       <c r="C361" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D361" t="s">
         <v>79</v>
@@ -14892,7 +15138,7 @@
         <v>14</v>
       </c>
       <c r="F361" t="s">
-        <v>1135</v>
+        <v>1170</v>
       </c>
       <c r="G361" t="s">
         <v>47</v>
@@ -14909,10 +15155,10 @@
     </row>
     <row r="362" spans="1:10">
       <c r="A362" t="s">
-        <v>1136</v>
+        <v>1171</v>
       </c>
       <c r="C362" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D362" t="s">
         <v>171</v>
@@ -14921,7 +15167,7 @@
         <v>14</v>
       </c>
       <c r="F362" t="s">
-        <v>1137</v>
+        <v>1172</v>
       </c>
       <c r="G362" t="s">
         <v>27</v>
@@ -14938,10 +15184,10 @@
     </row>
     <row r="363" spans="1:10">
       <c r="A363" t="s">
-        <v>1138</v>
+        <v>1173</v>
       </c>
       <c r="C363" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D363" t="s">
         <v>205</v>
@@ -14950,7 +15196,7 @@
         <v>14</v>
       </c>
       <c r="F363" t="s">
-        <v>1139</v>
+        <v>1174</v>
       </c>
       <c r="G363" t="s">
         <v>27</v>
@@ -14967,10 +15213,10 @@
     </row>
     <row r="364" spans="1:10">
       <c r="A364" t="s">
-        <v>1140</v>
+        <v>1175</v>
       </c>
       <c r="C364" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D364" t="s">
         <v>66</v>
@@ -14979,10 +15225,10 @@
         <v>14</v>
       </c>
       <c r="F364" t="s">
-        <v>1137</v>
+        <v>1172</v>
       </c>
       <c r="G364" t="s">
-        <v>1141</v>
+        <v>1176</v>
       </c>
       <c r="H364" t="s">
         <v>750</v>
@@ -14996,10 +15242,10 @@
     </row>
     <row r="365" spans="1:10">
       <c r="A365" t="s">
-        <v>1142</v>
+        <v>1177</v>
       </c>
       <c r="C365" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D365" t="s">
         <v>248</v>
@@ -15008,7 +15254,7 @@
         <v>14</v>
       </c>
       <c r="F365" t="s">
-        <v>1092</v>
+        <v>1126</v>
       </c>
       <c r="G365" t="s">
         <v>27</v>
@@ -15025,10 +15271,10 @@
     </row>
     <row r="366" spans="1:10">
       <c r="A366" t="s">
-        <v>1143</v>
+        <v>1178</v>
       </c>
       <c r="C366" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D366" t="s">
         <v>248</v>
@@ -15037,7 +15283,7 @@
         <v>14</v>
       </c>
       <c r="F366" t="s">
-        <v>1144</v>
+        <v>1179</v>
       </c>
       <c r="G366" t="s">
         <v>180</v>
@@ -15054,10 +15300,10 @@
     </row>
     <row r="367" spans="1:10">
       <c r="A367" t="s">
-        <v>1145</v>
+        <v>1180</v>
       </c>
       <c r="C367" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D367" t="s">
         <v>158</v>
@@ -15066,10 +15312,10 @@
         <v>14</v>
       </c>
       <c r="F367" t="s">
-        <v>1100</v>
+        <v>1134</v>
       </c>
       <c r="G367" t="s">
-        <v>1146</v>
+        <v>1181</v>
       </c>
       <c r="H367" t="s">
         <v>733</v>
@@ -15083,10 +15329,10 @@
     </row>
     <row r="368" spans="1:10">
       <c r="A368" t="s">
-        <v>1147</v>
+        <v>1182</v>
       </c>
       <c r="C368" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
       <c r="D368" t="s">
         <v>143</v>
@@ -15095,7 +15341,7 @@
         <v>14</v>
       </c>
       <c r="F368" t="s">
-        <v>1148</v>
+        <v>1183</v>
       </c>
       <c r="G368" t="s">
         <v>109</v>

</xml_diff>

<commit_message>
Exception handling : blank search. Modify Quests UI. Completed translation of 集会所 ★1 ~ ★2 quest information.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18920"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18927"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -847,7 +847,7 @@
     <t>도스팡고(ドスファンゴ) 1마리 수렵</t>
   </si>
   <si>
-    <t>블루팡고(ブルファンゴ) 3마리 토벌</t>
+    <t>불팡고(ブルファンゴ) 3마리 토벌</t>
   </si>
   <si>
     <t>ニャンター、はじめてのお使い</t>
@@ -1024,7 +1024,7 @@
     <t>숲의 팡고들</t>
   </si>
   <si>
-    <t>블루팡고(ブルファンゴ) 10마리 토벌</t>
+    <t>불팡고(ブルファンゴ) 10마리 토벌</t>
   </si>
   <si>
     <t>도스게네포스(ドスランボス)의 머리 파괴</t>
@@ -1267,10 +1267,10 @@
     <t>ブルファンゴを狩れ！</t>
   </si>
   <si>
-    <t>블루팡고를 사냥해라!</t>
-  </si>
-  <si>
-    <t>블루팡고(ブルファンゴ) 20마리 토벌</t>
+    <t>불팡고를 사냥해라!</t>
+  </si>
+  <si>
+    <t>불팡고(ブルファンゴ) 20마리 토벌</t>
   </si>
   <si>
     <t>毒怪鳥ゲリョスを追え！</t>
@@ -1972,10 +1972,10 @@
     <t>白昼のブルファンゴ討伐</t>
   </si>
   <si>
-    <t>대낮의 블루팡고 토벌</t>
-  </si>
-  <si>
-    <t>블루팡고(ブルファンゴ)를 10마리 이상 토벌하고 타임업 혹은 고양이택시티켓(ネコタクチケット) 납품</t>
+    <t>대낮의 불팡고 토벌</t>
+  </si>
+  <si>
+    <t>불팡고(ブルファンゴ)를 10마리 이상 토벌하고 타임업 혹은 고양이택시티켓(ネコタクチケット) 납품</t>
   </si>
   <si>
     <t>噴煙まとう王者</t>
@@ -1990,7 +1990,7 @@
     <t>再びキノコ探しで大もうけ！？</t>
   </si>
   <si>
-    <t>다시한번 버섯을 찾아서 큰 벌이!?</t>
+    <t>다시한번 버섯을 찾아서 큰벌이!?</t>
   </si>
   <si>
     <t>특산 버섯(特産キノコ) 10개 이상 납품 혹은 고양이택시티켓(ネコタクチケット) 납품</t>
@@ -3076,7 +3076,7 @@
     <t>예쁜 조개껍데기(きれいな貝殻) 10개 납품</t>
   </si>
   <si>
-    <t>블루팡고(ブルファンゴ) 8마리 토벌</t>
+    <t>불팡고(ブルファンゴ) 8마리 토벌</t>
   </si>
   <si>
     <t>龍識船強化！【水竜編】</t>
@@ -3931,8 +3931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J368"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="E233" sqref="E233"/>
+    <sheetView tabSelected="1" topLeftCell="B41" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Mistranslation correction. Add more categories in Quests. Completed translation of 集会所 ★3 quest information.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -2146,7 +2146,7 @@
     <t>ドス来い！真夜中の古代林</t>
   </si>
   <si>
-    <t>도스와라! 한밤중의 고대림</t>
+    <t>도스덤벼! 한밤중의 고대림</t>
   </si>
   <si>
     <t>混乱のホロロロホルルル</t>
@@ -2215,7 +2215,7 @@
     <t>廻り集いて回帰せん</t>
   </si>
   <si>
-    <t>돌고 모여서 회귀하다</t>
+    <t>돌고 울어서 회귀하리라</t>
   </si>
   <si>
     <t>샤갈마가라(シャガルマガラ) 1마리 토벌</t>
@@ -2278,7 +2278,7 @@
     <t>縄張りに進入するべからず</t>
   </si>
   <si>
-    <t>영역에 진입하지 말 것</t>
+    <t>영역에 진입하지 말지어니</t>
   </si>
   <si>
     <t>진오우가(ジンオウガ)의 등 파괴</t>
@@ -2425,7 +2425,7 @@
     <t>千刃、襲来</t>
   </si>
   <si>
-    <t>천인, 습래</t>
+    <t>천인, 내습</t>
   </si>
   <si>
     <t>天下分け目の大合戦</t>
@@ -3931,8 +3931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J368"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B41" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" topLeftCell="A209" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="B231" sqref="B231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Completed translation of 集会所 quest information. And completed the input into the database.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -613,7 +613,7 @@
     <t>고난도 : 아지랑이의 제국</t>
   </si>
   <si>
-    <t>테오・카스카토르(テオ・テスカトル) 토벌 혹은 격퇴</t>
+    <t>테오・테스카토르(テオ・テスカトル) 토벌 혹은 격퇴</t>
   </si>
   <si>
     <t>高難度：喧嘩の仲裁は村を救う</t>

</xml_diff>

<commit_message>
Completed translation of G★2 quest information. Mistranslation correction.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3592" uniqueCount="1179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3592" uniqueCount="1180">
   <si>
     <t>questName</t>
   </si>
@@ -106,10 +106,10 @@
     <t>マッカォの群れを討伐せよ！</t>
   </si>
   <si>
-    <t>마콰 무리를 토벌해라!</t>
-  </si>
-  <si>
-    <t>마콰(マッカォ) 10마리 토벌</t>
+    <t>마카오 무리를 토벌해라!</t>
+  </si>
+  <si>
+    <t>마카오(マッカォ) 10마리 토벌</t>
   </si>
   <si>
     <t>森の中のケルビ</t>
@@ -832,7 +832,7 @@
     <t>고대림의 정산 아이템 납품</t>
   </si>
   <si>
-    <t>도스마콰(ドスマッカォ) 수렵</t>
+    <t>도스마카오(ドスマッカォ) 수렵</t>
   </si>
   <si>
     <t>200z</t>
@@ -1036,7 +1036,7 @@
     <t>고대림의 망나니</t>
   </si>
   <si>
-    <t>마콰(マッカォ) 15마리 토벌</t>
+    <t>마카오(マッカォ) 15마리 토벌</t>
   </si>
   <si>
     <t>ゲネポス討伐作戦！</t>
@@ -1399,7 +1399,7 @@
     <t>재주좋은 꼬리에 매혹당해서</t>
   </si>
   <si>
-    <t>도스마콰(ドスマッカォ) 2마리 수렵</t>
+    <t>도스마카오(ドスマッカォ) 2마리 수렵</t>
   </si>
   <si>
     <t>용의눈물(竜のナミダ) 1개 납품</t>
@@ -1588,7 +1588,7 @@
     <t>도구룡의 머리파괴에 도전!</t>
   </si>
   <si>
-    <t>도스마콰(ドスマッカォ) 머리 파괴</t>
+    <t>도스마카오(ドスマッカォ) 머리 파괴</t>
   </si>
   <si>
     <t>火山の精算アイテム納品</t>
@@ -2407,7 +2407,7 @@
     <t>파랑과 녹색의 파상포위망</t>
   </si>
   <si>
-    <t>도스란포스(ドスランポス), 도스마콰(ドスマッカォ) 수렵</t>
+    <t>도스란포스(ドスランポス), 도스마카오(ドスマッカォ) 수렵</t>
   </si>
   <si>
     <t>高難度：天と地の怒り</t>
@@ -2500,6 +2500,9 @@
     <t>고난도 : 중갑충과 실력시험!</t>
   </si>
   <si>
+    <t>단차에 의한 다운을 5회 성공</t>
+  </si>
+  <si>
     <t>게넬・셀타스(ゲネル・セルタス) 1마리 수렵</t>
   </si>
   <si>
@@ -2563,10 +2566,10 @@
     <t>마을★7</t>
   </si>
   <si>
-    <t>도스마콰(ドスマッカォ) 1마리 수렵</t>
-  </si>
-  <si>
-    <t>도스마콰(ドスマッカォ)의 머리 파괴</t>
+    <t>도스마카오(ドスマッカォ) 1마리 수렵</t>
+  </si>
+  <si>
+    <t>도스마카오(ドスマッカォ)의 머리 파괴</t>
   </si>
   <si>
     <t>ぱっくん！テツカブラ</t>
@@ -2983,7 +2986,7 @@
     <t>날고 뛰어오르며 무아무중</t>
   </si>
   <si>
-    <t>케챠와챠(ケチャワチャ) 1마리와 도스마콰(ドスマッカォ) 1마리 수렵</t>
+    <t>케챠와챠(ケチャワチャ) 1마리와 도스마카오(ドスマッカォ) 1마리 수렵</t>
   </si>
   <si>
     <t>砂まみれですな</t>
@@ -3163,7 +3166,7 @@
     <t>嗚呼素晴らしき也、絞蛇竜</t>
   </si>
   <si>
-    <t>아아 훌륭하도다, 교사룡</t>
+    <t>아아 훌륭하니라, 교사룡</t>
   </si>
   <si>
     <t>가라라아쟈라(ガララアジャラ) 1마리 포획</t>
@@ -3931,8 +3934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J368"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A209" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="B231" sqref="B231"/>
+    <sheetView tabSelected="1" topLeftCell="A243" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="B324" sqref="B324"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11327,13 +11330,13 @@
         <v>719</v>
       </c>
       <c r="D239" t="s">
-        <v>143</v>
+        <v>827</v>
       </c>
       <c r="E239" t="s">
         <v>14</v>
       </c>
       <c r="F239" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="G239" t="s">
         <v>27</v>
@@ -11347,10 +11350,10 @@
     </row>
     <row r="240" spans="1:10">
       <c r="A240" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="B240" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="C240" t="s">
         <v>719</v>
@@ -11368,18 +11371,18 @@
         <v>27</v>
       </c>
       <c r="H240" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="I240" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
     </row>
     <row r="241" spans="1:10">
       <c r="A241" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="B241" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="C241" t="s">
         <v>719</v>
@@ -11405,10 +11408,10 @@
     </row>
     <row r="242" spans="1:10">
       <c r="A242" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="B242" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="C242" t="s">
         <v>719</v>
@@ -11437,10 +11440,10 @@
     </row>
     <row r="243" spans="1:10">
       <c r="A243" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="B243" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="C243" t="s">
         <v>719</v>
@@ -11461,15 +11464,15 @@
         <v>530</v>
       </c>
       <c r="I243" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
     </row>
     <row r="244" spans="1:10">
       <c r="A244" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="B244" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="C244" t="s">
         <v>719</v>
@@ -11490,7 +11493,7 @@
         <v>58</v>
       </c>
       <c r="I244" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="J244" t="s">
         <v>71</v>
@@ -11498,10 +11501,10 @@
     </row>
     <row r="245" spans="1:10">
       <c r="A245" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="B245" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="C245" t="s">
         <v>719</v>
@@ -11522,18 +11525,18 @@
         <v>735</v>
       </c>
       <c r="I245" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
     </row>
     <row r="246" spans="1:10">
       <c r="A246" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="B246" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="C246" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D246" t="s">
         <v>91</v>
@@ -11542,10 +11545,10 @@
         <v>14</v>
       </c>
       <c r="F246" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="G246" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="H246" t="s">
         <v>272</v>
@@ -11565,7 +11568,7 @@
         <v>329</v>
       </c>
       <c r="C247" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D247" t="s">
         <v>194</v>
@@ -11591,13 +11594,13 @@
     </row>
     <row r="248" spans="1:10">
       <c r="A248" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="B248" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="C248" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D248" t="s">
         <v>13</v>
@@ -11623,13 +11626,13 @@
     </row>
     <row r="249" spans="1:10">
       <c r="A249" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="B249" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="C249" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D249" t="s">
         <v>66</v>
@@ -11638,7 +11641,7 @@
         <v>14</v>
       </c>
       <c r="F249" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="G249" t="s">
         <v>27</v>
@@ -11655,13 +11658,13 @@
     </row>
     <row r="250" spans="1:10">
       <c r="A250" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="B250" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="C250" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D250" t="s">
         <v>66</v>
@@ -11687,13 +11690,13 @@
     </row>
     <row r="251" spans="1:10">
       <c r="A251" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="B251" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="C251" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D251" t="s">
         <v>143</v>
@@ -11719,13 +11722,13 @@
     </row>
     <row r="252" spans="1:10">
       <c r="A252" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="B252" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="C252" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D252" t="s">
         <v>91</v>
@@ -11751,13 +11754,13 @@
     </row>
     <row r="253" spans="1:10">
       <c r="A253" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="B253" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="C253" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D253" t="s">
         <v>66</v>
@@ -11766,7 +11769,7 @@
         <v>14</v>
       </c>
       <c r="F253" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="G253" t="s">
         <v>761</v>
@@ -11783,13 +11786,13 @@
     </row>
     <row r="254" spans="1:10">
       <c r="A254" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="B254" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="C254" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D254" t="s">
         <v>194</v>
@@ -11798,7 +11801,7 @@
         <v>14</v>
       </c>
       <c r="F254" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="G254" t="s">
         <v>109</v>
@@ -11807,7 +11810,7 @@
         <v>721</v>
       </c>
       <c r="I254" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="J254" t="s">
         <v>218</v>
@@ -11821,7 +11824,7 @@
         <v>312</v>
       </c>
       <c r="C255" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D255" t="s">
         <v>112</v>
@@ -11847,13 +11850,13 @@
     </row>
     <row r="256" spans="1:10">
       <c r="A256" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="B256" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="C256" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D256" t="s">
         <v>143</v>
@@ -11879,13 +11882,13 @@
     </row>
     <row r="257" spans="1:10">
       <c r="A257" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="B257" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="C257" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D257" t="s">
         <v>91</v>
@@ -11894,10 +11897,10 @@
         <v>14</v>
       </c>
       <c r="F257" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="G257" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="H257" t="s">
         <v>272</v>
@@ -11911,13 +11914,13 @@
     </row>
     <row r="258" spans="1:10">
       <c r="A258" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="B258" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="C258" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D258" t="s">
         <v>91</v>
@@ -11943,13 +11946,13 @@
     </row>
     <row r="259" spans="1:10">
       <c r="A259" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="B259" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="C259" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D259" t="s">
         <v>13</v>
@@ -11958,10 +11961,10 @@
         <v>14</v>
       </c>
       <c r="F259" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="G259" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="H259" t="s">
         <v>180</v>
@@ -11975,13 +11978,13 @@
     </row>
     <row r="260" spans="1:10">
       <c r="A260" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="B260" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="C260" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D260" t="s">
         <v>91</v>
@@ -11990,7 +11993,7 @@
         <v>14</v>
       </c>
       <c r="F260" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="G260" t="s">
         <v>27</v>
@@ -12007,13 +12010,13 @@
     </row>
     <row r="261" spans="1:10">
       <c r="A261" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="B261" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="C261" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D261" t="s">
         <v>91</v>
@@ -12022,7 +12025,7 @@
         <v>14</v>
       </c>
       <c r="F261" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="G261" t="s">
         <v>27</v>
@@ -12045,7 +12048,7 @@
         <v>298</v>
       </c>
       <c r="C262" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D262" t="s">
         <v>53</v>
@@ -12077,7 +12080,7 @@
         <v>348</v>
       </c>
       <c r="C263" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D263" t="s">
         <v>13</v>
@@ -12103,13 +12106,13 @@
     </row>
     <row r="264" spans="1:10">
       <c r="A264" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B264" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C264" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D264" t="s">
         <v>183</v>
@@ -12118,7 +12121,7 @@
         <v>14</v>
       </c>
       <c r="F264" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="G264" t="s">
         <v>47</v>
@@ -12135,13 +12138,13 @@
     </row>
     <row r="265" spans="1:10">
       <c r="A265" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="B265" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="C265" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D265" t="s">
         <v>66</v>
@@ -12150,7 +12153,7 @@
         <v>14</v>
       </c>
       <c r="F265" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="G265" t="s">
         <v>303</v>
@@ -12167,13 +12170,13 @@
     </row>
     <row r="266" spans="1:10">
       <c r="A266" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="B266" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="C266" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D266" t="s">
         <v>112</v>
@@ -12185,7 +12188,7 @@
         <v>413</v>
       </c>
       <c r="G266" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="H266" t="s">
         <v>18</v>
@@ -12199,13 +12202,13 @@
     </row>
     <row r="267" spans="1:10">
       <c r="A267" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="B267" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="C267" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D267" t="s">
         <v>91</v>
@@ -12214,7 +12217,7 @@
         <v>14</v>
       </c>
       <c r="F267" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="G267" t="s">
         <v>27</v>
@@ -12231,13 +12234,13 @@
     </row>
     <row r="268" spans="1:10">
       <c r="A268" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="B268" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="C268" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D268" t="s">
         <v>91</v>
@@ -12269,7 +12272,7 @@
         <v>327</v>
       </c>
       <c r="C269" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D269" t="s">
         <v>183</v>
@@ -12295,13 +12298,13 @@
     </row>
     <row r="270" spans="1:10">
       <c r="A270" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="B270" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="C270" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D270" t="s">
         <v>91</v>
@@ -12310,7 +12313,7 @@
         <v>14</v>
       </c>
       <c r="F270" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="G270" t="s">
         <v>55</v>
@@ -12327,13 +12330,13 @@
     </row>
     <row r="271" spans="1:10">
       <c r="A271" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="B271" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="C271" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D271" t="s">
         <v>112</v>
@@ -12342,10 +12345,10 @@
         <v>14</v>
       </c>
       <c r="F271" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="G271" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="H271" t="s">
         <v>272</v>
@@ -12359,13 +12362,13 @@
     </row>
     <row r="272" spans="1:10">
       <c r="A272" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="B272" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="C272" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D272" t="s">
         <v>91</v>
@@ -12374,7 +12377,7 @@
         <v>14</v>
       </c>
       <c r="F272" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="G272" t="s">
         <v>439</v>
@@ -12391,13 +12394,13 @@
     </row>
     <row r="273" spans="1:10">
       <c r="A273" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="B273" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="C273" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D273" t="s">
         <v>66</v>
@@ -12406,10 +12409,10 @@
         <v>14</v>
       </c>
       <c r="F273" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="G273" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="H273" t="s">
         <v>272</v>
@@ -12423,13 +12426,13 @@
     </row>
     <row r="274" spans="1:10">
       <c r="A274" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="B274" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="C274" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D274" t="s">
         <v>45</v>
@@ -12438,10 +12441,10 @@
         <v>14</v>
       </c>
       <c r="F274" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="G274" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="H274" t="s">
         <v>272</v>
@@ -12455,13 +12458,13 @@
     </row>
     <row r="275" spans="1:10">
       <c r="A275" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="B275" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="C275" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D275" t="s">
         <v>53</v>
@@ -12470,10 +12473,10 @@
         <v>14</v>
       </c>
       <c r="F275" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="G275" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="H275" t="s">
         <v>180</v>
@@ -12487,13 +12490,13 @@
     </row>
     <row r="276" spans="1:10">
       <c r="A276" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="B276" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="C276" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D276" t="s">
         <v>45</v>
@@ -12502,7 +12505,7 @@
         <v>14</v>
       </c>
       <c r="F276" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="G276" t="s">
         <v>109</v>
@@ -12519,13 +12522,13 @@
     </row>
     <row r="277" spans="1:10">
       <c r="A277" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="B277" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="C277" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D277" t="s">
         <v>45</v>
@@ -12551,13 +12554,13 @@
     </row>
     <row r="278" spans="1:10">
       <c r="A278" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="B278" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="C278" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D278" t="s">
         <v>194</v>
@@ -12566,7 +12569,7 @@
         <v>14</v>
       </c>
       <c r="F278" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="G278" t="s">
         <v>362</v>
@@ -12583,13 +12586,13 @@
     </row>
     <row r="279" spans="1:10">
       <c r="A279" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="B279" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="C279" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D279" t="s">
         <v>13</v>
@@ -12598,16 +12601,16 @@
         <v>14</v>
       </c>
       <c r="F279" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="G279" t="s">
         <v>27</v>
       </c>
       <c r="H279" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="I279" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="J279" t="s">
         <v>17</v>
@@ -12615,13 +12618,13 @@
     </row>
     <row r="280" spans="1:10">
       <c r="A280" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="B280" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="C280" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D280" t="s">
         <v>143</v>
@@ -12647,13 +12650,13 @@
     </row>
     <row r="281" spans="1:10">
       <c r="A281" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="B281" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="C281" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D281" t="s">
         <v>53</v>
@@ -12679,13 +12682,13 @@
     </row>
     <row r="282" spans="1:10">
       <c r="A282" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B282" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="C282" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D282" t="s">
         <v>66</v>
@@ -12717,7 +12720,7 @@
         <v>541</v>
       </c>
       <c r="C283" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D283" t="s">
         <v>204</v>
@@ -12743,13 +12746,13 @@
     </row>
     <row r="284" spans="1:10">
       <c r="A284" t="s">
+        <v>941</v>
+      </c>
+      <c r="B284" t="s">
+        <v>942</v>
+      </c>
+      <c r="C284" t="s">
         <v>940</v>
-      </c>
-      <c r="B284" t="s">
-        <v>941</v>
-      </c>
-      <c r="C284" t="s">
-        <v>939</v>
       </c>
       <c r="D284" t="s">
         <v>79</v>
@@ -12758,7 +12761,7 @@
         <v>14</v>
       </c>
       <c r="F284" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="G284" t="s">
         <v>609</v>
@@ -12775,13 +12778,13 @@
     </row>
     <row r="285" spans="1:10">
       <c r="A285" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="B285" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="C285" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D285" t="s">
         <v>86</v>
@@ -12807,13 +12810,13 @@
     </row>
     <row r="286" spans="1:10">
       <c r="A286" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="B286" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="C286" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D286" t="s">
         <v>204</v>
@@ -12822,7 +12825,7 @@
         <v>14</v>
       </c>
       <c r="F286" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="G286" t="s">
         <v>27</v>
@@ -12839,13 +12842,13 @@
     </row>
     <row r="287" spans="1:10">
       <c r="A287" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="B287" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="C287" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D287" t="s">
         <v>13</v>
@@ -12854,10 +12857,10 @@
         <v>14</v>
       </c>
       <c r="F287" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="G287" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="H287" t="s">
         <v>18</v>
@@ -12871,13 +12874,13 @@
     </row>
     <row r="288" spans="1:10">
       <c r="A288" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="B288" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="C288" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D288" t="s">
         <v>66</v>
@@ -12903,13 +12906,13 @@
     </row>
     <row r="289" spans="1:10">
       <c r="A289" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="B289" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="C289" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D289" t="s">
         <v>53</v>
@@ -12921,7 +12924,7 @@
         <v>617</v>
       </c>
       <c r="G289" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="H289" t="s">
         <v>18</v>
@@ -12935,13 +12938,13 @@
     </row>
     <row r="290" spans="1:10">
       <c r="A290" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="B290" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="C290" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D290" t="s">
         <v>183</v>
@@ -12950,16 +12953,16 @@
         <v>14</v>
       </c>
       <c r="F290" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="G290" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="H290" t="s">
         <v>735</v>
       </c>
       <c r="I290" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="J290" t="s">
         <v>82</v>
@@ -12967,13 +12970,13 @@
     </row>
     <row r="291" spans="1:10">
       <c r="A291" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="B291" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="C291" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D291" t="s">
         <v>79</v>
@@ -12985,7 +12988,7 @@
         <v>682</v>
       </c>
       <c r="G291" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="H291" t="s">
         <v>23</v>
@@ -12999,13 +13002,13 @@
     </row>
     <row r="292" spans="1:10">
       <c r="A292" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="B292" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="C292" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D292" t="s">
         <v>112</v>
@@ -13014,7 +13017,7 @@
         <v>14</v>
       </c>
       <c r="F292" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="G292" t="s">
         <v>27</v>
@@ -13031,13 +13034,13 @@
     </row>
     <row r="293" spans="1:10">
       <c r="A293" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="B293" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="C293" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D293" t="s">
         <v>79</v>
@@ -13046,7 +13049,7 @@
         <v>14</v>
       </c>
       <c r="F293" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="G293" t="s">
         <v>27</v>
@@ -13069,7 +13072,7 @@
         <v>453</v>
       </c>
       <c r="C294" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D294" t="s">
         <v>158</v>
@@ -13095,13 +13098,13 @@
     </row>
     <row r="295" spans="1:10">
       <c r="A295" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="B295" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="C295" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D295" t="s">
         <v>79</v>
@@ -13127,13 +13130,13 @@
     </row>
     <row r="296" spans="1:10">
       <c r="A296" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="B296" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="C296" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D296" t="s">
         <v>204</v>
@@ -13142,7 +13145,7 @@
         <v>14</v>
       </c>
       <c r="F296" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="G296" t="s">
         <v>47</v>
@@ -13165,7 +13168,7 @@
         <v>399</v>
       </c>
       <c r="C297" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D297" t="s">
         <v>247</v>
@@ -13191,13 +13194,13 @@
     </row>
     <row r="298" spans="1:10">
       <c r="A298" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="B298" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="C298" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D298" t="s">
         <v>91</v>
@@ -13209,7 +13212,7 @@
         <v>582</v>
       </c>
       <c r="G298" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="H298" t="s">
         <v>552</v>
@@ -13223,13 +13226,13 @@
     </row>
     <row r="299" spans="1:10">
       <c r="A299" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="B299" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="C299" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D299" t="s">
         <v>204</v>
@@ -13241,13 +13244,13 @@
         <v>698</v>
       </c>
       <c r="G299" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="H299" t="s">
         <v>721</v>
       </c>
       <c r="I299" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="J299" t="s">
         <v>82</v>
@@ -13255,13 +13258,13 @@
     </row>
     <row r="300" spans="1:10">
       <c r="A300" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="B300" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="C300" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D300" t="s">
         <v>122</v>
@@ -13279,7 +13282,7 @@
         <v>721</v>
       </c>
       <c r="I300" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="J300" t="s">
         <v>82</v>
@@ -13287,13 +13290,13 @@
     </row>
     <row r="301" spans="1:10">
       <c r="A301" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B301" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C301" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D301" t="s">
         <v>247</v>
@@ -13302,7 +13305,7 @@
         <v>14</v>
       </c>
       <c r="F301" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="G301" t="s">
         <v>109</v>
@@ -13319,13 +13322,13 @@
     </row>
     <row r="302" spans="1:10">
       <c r="A302" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="B302" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="C302" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D302" t="s">
         <v>45</v>
@@ -13334,7 +13337,7 @@
         <v>14</v>
       </c>
       <c r="F302" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="G302" t="s">
         <v>362</v>
@@ -13351,13 +13354,13 @@
     </row>
     <row r="303" spans="1:10">
       <c r="A303" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="B303" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="C303" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D303" t="s">
         <v>194</v>
@@ -13366,7 +13369,7 @@
         <v>14</v>
       </c>
       <c r="F303" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="G303" t="s">
         <v>47</v>
@@ -13383,13 +13386,13 @@
     </row>
     <row r="304" spans="1:10">
       <c r="A304" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="B304" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="C304" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D304" t="s">
         <v>247</v>
@@ -13398,7 +13401,7 @@
         <v>14</v>
       </c>
       <c r="F304" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="G304" t="s">
         <v>362</v>
@@ -13415,13 +13418,13 @@
     </row>
     <row r="305" spans="1:10">
       <c r="A305" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="B305" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="C305" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D305" t="s">
         <v>158</v>
@@ -13430,7 +13433,7 @@
         <v>14</v>
       </c>
       <c r="F305" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="G305" t="s">
         <v>47</v>
@@ -13439,7 +13442,7 @@
         <v>735</v>
       </c>
       <c r="I305" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="J305" t="s">
         <v>50</v>
@@ -13447,13 +13450,13 @@
     </row>
     <row r="306" spans="1:10">
       <c r="A306" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="B306" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="C306" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D306" t="s">
         <v>66</v>
@@ -13465,7 +13468,7 @@
         <v>504</v>
       </c>
       <c r="G306" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="H306" t="s">
         <v>180</v>
@@ -13479,13 +13482,13 @@
     </row>
     <row r="307" spans="1:10">
       <c r="A307" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="B307" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="C307" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D307" t="s">
         <v>86</v>
@@ -13494,10 +13497,10 @@
         <v>14</v>
       </c>
       <c r="F307" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="G307" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="H307" t="s">
         <v>180</v>
@@ -13511,13 +13514,13 @@
     </row>
     <row r="308" spans="1:10">
       <c r="A308" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="B308" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="C308" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D308" t="s">
         <v>91</v>
@@ -13543,13 +13546,13 @@
     </row>
     <row r="309" spans="1:10">
       <c r="A309" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="B309" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="C309" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D309" t="s">
         <v>66</v>
@@ -13561,7 +13564,7 @@
         <v>565</v>
       </c>
       <c r="G309" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="H309" t="s">
         <v>180</v>
@@ -13575,13 +13578,13 @@
     </row>
     <row r="310" spans="1:10">
       <c r="A310" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="B310" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="C310" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D310" t="s">
         <v>143</v>
@@ -13590,7 +13593,7 @@
         <v>14</v>
       </c>
       <c r="F310" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="G310" t="s">
         <v>27</v>
@@ -13607,13 +13610,13 @@
     </row>
     <row r="311" spans="1:10">
       <c r="A311" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="B311" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="C311" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D311" t="s">
         <v>91</v>
@@ -13622,10 +13625,10 @@
         <v>14</v>
       </c>
       <c r="F311" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="G311" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="H311" t="s">
         <v>18</v>
@@ -13639,13 +13642,13 @@
     </row>
     <row r="312" spans="1:10">
       <c r="A312" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="B312" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="C312" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D312" t="s">
         <v>79</v>
@@ -13654,10 +13657,10 @@
         <v>14</v>
       </c>
       <c r="F312" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="G312" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="H312" t="s">
         <v>18</v>
@@ -13671,13 +13674,13 @@
     </row>
     <row r="313" spans="1:10">
       <c r="A313" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="B313" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="C313" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D313" t="s">
         <v>91</v>
@@ -13686,7 +13689,7 @@
         <v>14</v>
       </c>
       <c r="F313" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="G313" t="s">
         <v>27</v>
@@ -13703,13 +13706,13 @@
     </row>
     <row r="314" spans="1:10">
       <c r="A314" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="B314" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="C314" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D314" t="s">
         <v>112</v>
@@ -13721,7 +13724,7 @@
         <v>544</v>
       </c>
       <c r="G314" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="H314" t="s">
         <v>23</v>
@@ -13735,13 +13738,13 @@
     </row>
     <row r="315" spans="1:10">
       <c r="A315" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="B315" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="C315" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D315" t="s">
         <v>91</v>
@@ -13750,7 +13753,7 @@
         <v>14</v>
       </c>
       <c r="F315" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="G315" t="s">
         <v>27</v>
@@ -13767,13 +13770,13 @@
     </row>
     <row r="316" spans="1:10">
       <c r="A316" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="B316" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="C316" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D316" t="s">
         <v>91</v>
@@ -13799,13 +13802,13 @@
     </row>
     <row r="317" spans="1:10">
       <c r="A317" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="B317" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="C317" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D317" t="s">
         <v>122</v>
@@ -13831,13 +13834,13 @@
     </row>
     <row r="318" spans="1:10">
       <c r="A318" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="B318" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="C318" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D318" t="s">
         <v>158</v>
@@ -13846,10 +13849,10 @@
         <v>14</v>
       </c>
       <c r="F318" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="G318" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="H318" t="s">
         <v>23</v>
@@ -13863,13 +13866,13 @@
     </row>
     <row r="319" spans="1:10">
       <c r="A319" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="B319" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="C319" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D319" t="s">
         <v>86</v>
@@ -13878,10 +13881,10 @@
         <v>14</v>
       </c>
       <c r="F319" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="G319" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="H319" t="s">
         <v>552</v>
@@ -13895,13 +13898,13 @@
     </row>
     <row r="320" spans="1:10">
       <c r="A320" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="B320" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="C320" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D320" t="s">
         <v>79</v>
@@ -13910,10 +13913,10 @@
         <v>14</v>
       </c>
       <c r="F320" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="G320" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="H320" t="s">
         <v>18</v>
@@ -13927,13 +13930,13 @@
     </row>
     <row r="321" spans="1:10">
       <c r="A321" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="B321" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="C321" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D321" t="s">
         <v>112</v>
@@ -13942,10 +13945,10 @@
         <v>14</v>
       </c>
       <c r="F321" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="G321" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="H321" t="s">
         <v>180</v>
@@ -13959,13 +13962,13 @@
     </row>
     <row r="322" spans="1:10">
       <c r="A322" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="B322" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="C322" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D322" t="s">
         <v>143</v>
@@ -13974,7 +13977,7 @@
         <v>14</v>
       </c>
       <c r="F322" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="G322" t="s">
         <v>27</v>
@@ -13991,13 +13994,13 @@
     </row>
     <row r="323" spans="1:10">
       <c r="A323" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="B323" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="C323" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D323" t="s">
         <v>143</v>
@@ -14006,7 +14009,7 @@
         <v>14</v>
       </c>
       <c r="F323" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="G323" t="s">
         <v>109</v>
@@ -14023,13 +14026,13 @@
     </row>
     <row r="324" spans="1:10">
       <c r="A324" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="B324" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="C324" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="D324" t="s">
         <v>158</v>
@@ -14038,7 +14041,7 @@
         <v>14</v>
       </c>
       <c r="F324" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="G324" t="s">
         <v>362</v>
@@ -14047,7 +14050,7 @@
         <v>735</v>
       </c>
       <c r="I324" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="J324" t="s">
         <v>228</v>
@@ -14055,13 +14058,13 @@
     </row>
     <row r="325" spans="1:10">
       <c r="A325" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="B325" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="C325" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D325" t="s">
         <v>66</v>
@@ -14073,7 +14076,7 @@
         <v>113</v>
       </c>
       <c r="G325" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="H325" t="s">
         <v>69</v>
@@ -14087,13 +14090,13 @@
     </row>
     <row r="326" spans="1:10">
       <c r="A326" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="B326" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="C326" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D326" t="s">
         <v>183</v>
@@ -14111,7 +14114,7 @@
         <v>735</v>
       </c>
       <c r="I326" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="J326" t="s">
         <v>17</v>
@@ -14119,13 +14122,13 @@
     </row>
     <row r="327" spans="1:10">
       <c r="A327" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="B327" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="C327" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D327" t="s">
         <v>86</v>
@@ -14134,7 +14137,7 @@
         <v>14</v>
       </c>
       <c r="F327" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="G327" t="s">
         <v>27</v>
@@ -14151,13 +14154,13 @@
     </row>
     <row r="328" spans="1:10">
       <c r="A328" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="B328" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="C328" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D328" t="s">
         <v>53</v>
@@ -14175,7 +14178,7 @@
         <v>735</v>
       </c>
       <c r="I328" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="J328" t="s">
         <v>17</v>
@@ -14183,13 +14186,13 @@
     </row>
     <row r="329" spans="1:10">
       <c r="A329" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="B329" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="C329" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D329" t="s">
         <v>13</v>
@@ -14215,13 +14218,13 @@
     </row>
     <row r="330" spans="1:10">
       <c r="A330" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="B330" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="C330" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D330" t="s">
         <v>86</v>
@@ -14230,16 +14233,16 @@
         <v>14</v>
       </c>
       <c r="F330" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="G330" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="H330" t="s">
         <v>228</v>
       </c>
       <c r="I330" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="J330" t="s">
         <v>441</v>
@@ -14247,13 +14250,13 @@
     </row>
     <row r="331" spans="1:10">
       <c r="A331" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="B331" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="C331" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D331" t="s">
         <v>91</v>
@@ -14262,10 +14265,10 @@
         <v>14</v>
       </c>
       <c r="F331" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="G331" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="H331" t="s">
         <v>48</v>
@@ -14279,13 +14282,13 @@
     </row>
     <row r="332" spans="1:10">
       <c r="A332" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="B332" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="C332" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D332" t="s">
         <v>79</v>
@@ -14297,7 +14300,7 @@
         <v>258</v>
       </c>
       <c r="G332" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="H332" t="s">
         <v>735</v>
@@ -14311,13 +14314,13 @@
     </row>
     <row r="333" spans="1:10">
       <c r="A333" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="B333" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="C333" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D333" t="s">
         <v>79</v>
@@ -14326,10 +14329,10 @@
         <v>14</v>
       </c>
       <c r="F333" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="G333" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="H333" t="s">
         <v>721</v>
@@ -14343,13 +14346,13 @@
     </row>
     <row r="334" spans="1:10">
       <c r="A334" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="B334" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="C334" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D334" t="s">
         <v>86</v>
@@ -14375,13 +14378,13 @@
     </row>
     <row r="335" spans="1:10">
       <c r="A335" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="B335" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="C335" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D335" t="s">
         <v>183</v>
@@ -14390,7 +14393,7 @@
         <v>14</v>
       </c>
       <c r="F335" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="G335" t="s">
         <v>250</v>
@@ -14407,13 +14410,13 @@
     </row>
     <row r="336" spans="1:10">
       <c r="A336" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="B336" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="C336" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D336" t="s">
         <v>194</v>
@@ -14422,7 +14425,7 @@
         <v>14</v>
       </c>
       <c r="F336" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="G336" t="s">
         <v>109</v>
@@ -14431,7 +14434,7 @@
         <v>48</v>
       </c>
       <c r="I336" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="J336" t="s">
         <v>441</v>
@@ -14439,13 +14442,13 @@
     </row>
     <row r="337" spans="1:10">
       <c r="A337" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="B337" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="C337" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D337" t="s">
         <v>122</v>
@@ -14454,10 +14457,10 @@
         <v>14</v>
       </c>
       <c r="F337" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="G337" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="H337" t="s">
         <v>48</v>
@@ -14471,13 +14474,13 @@
     </row>
     <row r="338" spans="1:10">
       <c r="A338" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="B338" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="C338" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D338" t="s">
         <v>204</v>
@@ -14503,13 +14506,13 @@
     </row>
     <row r="339" spans="1:10">
       <c r="A339" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="B339" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="C339" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D339" t="s">
         <v>13</v>
@@ -14527,7 +14530,7 @@
         <v>240</v>
       </c>
       <c r="I339" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="J339" t="s">
         <v>58</v>
@@ -14535,13 +14538,13 @@
     </row>
     <row r="340" spans="1:10">
       <c r="A340" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="B340" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="C340" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D340" t="s">
         <v>91</v>
@@ -14550,10 +14553,10 @@
         <v>14</v>
       </c>
       <c r="F340" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="G340" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="H340" t="s">
         <v>735</v>
@@ -14567,13 +14570,13 @@
     </row>
     <row r="341" spans="1:10">
       <c r="A341" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B341" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="C341" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D341" t="s">
         <v>45</v>
@@ -14585,13 +14588,13 @@
         <v>54</v>
       </c>
       <c r="G341" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="H341" t="s">
         <v>228</v>
       </c>
       <c r="I341" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="J341" t="s">
         <v>441</v>
@@ -14599,13 +14602,13 @@
     </row>
     <row r="342" spans="1:10">
       <c r="A342" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="B342" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="C342" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D342" t="s">
         <v>91</v>
@@ -14631,13 +14634,13 @@
     </row>
     <row r="343" spans="1:10">
       <c r="A343" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="B343" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="C343" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D343" t="s">
         <v>91</v>
@@ -14649,7 +14652,7 @@
         <v>250</v>
       </c>
       <c r="G343" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="H343" t="s">
         <v>721</v>
@@ -14663,13 +14666,13 @@
     </row>
     <row r="344" spans="1:10">
       <c r="A344" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="B344" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="C344" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D344" t="s">
         <v>79</v>
@@ -14695,13 +14698,13 @@
     </row>
     <row r="345" spans="1:10">
       <c r="A345" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="B345" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="C345" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D345" t="s">
         <v>112</v>
@@ -14710,7 +14713,7 @@
         <v>14</v>
       </c>
       <c r="F345" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="G345" t="s">
         <v>362</v>
@@ -14727,13 +14730,13 @@
     </row>
     <row r="346" spans="1:10">
       <c r="A346" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="B346" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="C346" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D346" t="s">
         <v>194</v>
@@ -14745,7 +14748,7 @@
         <v>54</v>
       </c>
       <c r="G346" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="H346" t="s">
         <v>114</v>
@@ -14759,13 +14762,13 @@
     </row>
     <row r="347" spans="1:10">
       <c r="A347" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="B347" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="C347" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D347" t="s">
         <v>122</v>
@@ -14774,7 +14777,7 @@
         <v>14</v>
       </c>
       <c r="F347" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="G347" t="s">
         <v>27</v>
@@ -14791,13 +14794,13 @@
     </row>
     <row r="348" spans="1:10">
       <c r="A348" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="B348" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="C348" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D348" t="s">
         <v>112</v>
@@ -14806,10 +14809,10 @@
         <v>14</v>
       </c>
       <c r="F348" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="G348" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="H348" t="s">
         <v>240</v>
@@ -14823,13 +14826,13 @@
     </row>
     <row r="349" spans="1:10">
       <c r="A349" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="B349" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="C349" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D349" t="s">
         <v>143</v>
@@ -14838,10 +14841,10 @@
         <v>14</v>
       </c>
       <c r="F349" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="G349" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="H349" t="s">
         <v>240</v>
@@ -14855,13 +14858,13 @@
     </row>
     <row r="350" spans="1:10">
       <c r="A350" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="B350" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="C350" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D350" t="s">
         <v>45</v>
@@ -14873,13 +14876,13 @@
         <v>663</v>
       </c>
       <c r="G350" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="H350" t="s">
         <v>735</v>
       </c>
       <c r="I350" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="J350" t="s">
         <v>441</v>
@@ -14887,13 +14890,13 @@
     </row>
     <row r="351" spans="1:10">
       <c r="A351" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="B351" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="C351" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D351" t="s">
         <v>91</v>
@@ -14911,7 +14914,7 @@
         <v>735</v>
       </c>
       <c r="I351" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="J351" t="s">
         <v>17</v>
@@ -14919,13 +14922,13 @@
     </row>
     <row r="352" spans="1:10">
       <c r="A352" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="B352" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="C352" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D352" t="s">
         <v>122</v>
@@ -14951,13 +14954,13 @@
     </row>
     <row r="353" spans="1:10">
       <c r="A353" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="B353" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="C353" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D353" t="s">
         <v>112</v>
@@ -14975,7 +14978,7 @@
         <v>735</v>
       </c>
       <c r="I353" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="J353" t="s">
         <v>17</v>
@@ -14983,13 +14986,13 @@
     </row>
     <row r="354" spans="1:10">
       <c r="A354" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="B354" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="C354" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D354" t="s">
         <v>86</v>
@@ -14998,10 +15001,10 @@
         <v>14</v>
       </c>
       <c r="F354" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="G354" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="H354" t="s">
         <v>69</v>
@@ -15015,13 +15018,13 @@
     </row>
     <row r="355" spans="1:10">
       <c r="A355" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="B355" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C355" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D355" t="s">
         <v>247</v>
@@ -15030,7 +15033,7 @@
         <v>14</v>
       </c>
       <c r="F355" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="G355" t="s">
         <v>27</v>
@@ -15047,13 +15050,13 @@
     </row>
     <row r="356" spans="1:10">
       <c r="A356" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="B356" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="C356" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D356" t="s">
         <v>194</v>
@@ -15062,7 +15065,7 @@
         <v>14</v>
       </c>
       <c r="F356" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="G356" t="s">
         <v>27</v>
@@ -15079,13 +15082,13 @@
     </row>
     <row r="357" spans="1:10">
       <c r="A357" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="B357" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="C357" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D357" t="s">
         <v>79</v>
@@ -15094,7 +15097,7 @@
         <v>14</v>
       </c>
       <c r="F357" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="G357" t="s">
         <v>47</v>
@@ -15111,13 +15114,13 @@
     </row>
     <row r="358" spans="1:10">
       <c r="A358" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="B358" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="C358" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D358" t="s">
         <v>79</v>
@@ -15129,13 +15132,13 @@
         <v>675</v>
       </c>
       <c r="G358" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="H358" t="s">
         <v>735</v>
       </c>
       <c r="I358" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="J358" t="s">
         <v>441</v>
@@ -15146,10 +15149,10 @@
         <v>141</v>
       </c>
       <c r="B359" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="C359" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D359" t="s">
         <v>143</v>
@@ -15161,13 +15164,13 @@
         <v>816</v>
       </c>
       <c r="G359" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="H359" t="s">
         <v>735</v>
       </c>
       <c r="I359" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="J359" t="s">
         <v>441</v>
@@ -15175,13 +15178,13 @@
     </row>
     <row r="360" spans="1:10">
       <c r="A360" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="B360" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="C360" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D360" t="s">
         <v>204</v>
@@ -15190,7 +15193,7 @@
         <v>14</v>
       </c>
       <c r="F360" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="G360" t="s">
         <v>47</v>
@@ -15199,7 +15202,7 @@
         <v>228</v>
       </c>
       <c r="I360" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="J360" t="s">
         <v>50</v>
@@ -15207,13 +15210,13 @@
     </row>
     <row r="361" spans="1:10">
       <c r="A361" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="B361" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="C361" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D361" t="s">
         <v>79</v>
@@ -15222,7 +15225,7 @@
         <v>14</v>
       </c>
       <c r="F361" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="G361" t="s">
         <v>47</v>
@@ -15239,13 +15242,13 @@
     </row>
     <row r="362" spans="1:10">
       <c r="A362" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="B362" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="C362" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D362" t="s">
         <v>13</v>
@@ -15263,7 +15266,7 @@
         <v>735</v>
       </c>
       <c r="I362" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="J362" t="s">
         <v>17</v>
@@ -15271,13 +15274,13 @@
     </row>
     <row r="363" spans="1:10">
       <c r="A363" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="B363" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="C363" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D363" t="s">
         <v>204</v>
@@ -15286,7 +15289,7 @@
         <v>14</v>
       </c>
       <c r="F363" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="G363" t="s">
         <v>27</v>
@@ -15303,13 +15306,13 @@
     </row>
     <row r="364" spans="1:10">
       <c r="A364" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="B364" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="C364" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D364" t="s">
         <v>66</v>
@@ -15321,13 +15324,13 @@
         <v>787</v>
       </c>
       <c r="G364" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="H364" t="s">
         <v>735</v>
       </c>
       <c r="I364" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="J364" t="s">
         <v>441</v>
@@ -15335,13 +15338,13 @@
     </row>
     <row r="365" spans="1:10">
       <c r="A365" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="B365" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="C365" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D365" t="s">
         <v>247</v>
@@ -15350,7 +15353,7 @@
         <v>14</v>
       </c>
       <c r="F365" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="G365" t="s">
         <v>27</v>
@@ -15367,13 +15370,13 @@
     </row>
     <row r="366" spans="1:10">
       <c r="A366" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="B366" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="C366" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D366" t="s">
         <v>247</v>
@@ -15399,13 +15402,13 @@
     </row>
     <row r="367" spans="1:10">
       <c r="A367" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="B367" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="C367" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D367" t="s">
         <v>158</v>
@@ -15417,7 +15420,7 @@
         <v>667</v>
       </c>
       <c r="G367" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="H367" t="s">
         <v>721</v>
@@ -15431,13 +15434,13 @@
     </row>
     <row r="368" spans="1:10">
       <c r="A368" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="B368" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="C368" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D368" t="s">
         <v>143</v>
@@ -15446,7 +15449,7 @@
         <v>14</v>
       </c>
       <c r="F368" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="G368" t="s">
         <v>109</v>

</xml_diff>

<commit_message>
Add keys to the model. Edit typo.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19007"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3592" uniqueCount="1180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3622" uniqueCount="1189">
   <si>
     <t>questName</t>
   </si>
@@ -2041,7 +2041,7 @@
     <t>淡紅の泡狐がたゆたうか</t>
   </si>
   <si>
-    <t>담홍의 호호가 흔들거리는가</t>
+    <t>담홍의 포호가 흔들거리는가</t>
   </si>
   <si>
     <t>타마미츠네(タマミツネ) 1마리 수렵</t>
@@ -2926,7 +2926,7 @@
     <t>龍識船強化！【迅竜編】</t>
   </si>
   <si>
-    <t>욕식선강화! [신룡편]</t>
+    <t>용식선강화! [신룡편]</t>
   </si>
   <si>
     <t>나루가크루가(ナルガクルガ) 1마리 수렵</t>
@@ -3557,6 +3557,33 @@
   </si>
   <si>
     <t>네르스큐라(ネルスキュラ) 2마리 수렵</t>
+  </si>
+  <si>
+    <t>跳躍のアウトロー</t>
+  </si>
+  <si>
+    <t>도약의 무법자</t>
+  </si>
+  <si>
+    <t>마카오(マッカォ) 5마리 토벌</t>
+  </si>
+  <si>
+    <t>古代林の大怪鳥</t>
+  </si>
+  <si>
+    <t>고대림의 대괴조</t>
+  </si>
+  <si>
+    <t>고대나무의 열매(古代木の実) 2개 납품</t>
+  </si>
+  <si>
+    <t>鬼面狩人を威す</t>
+  </si>
+  <si>
+    <t>귀면수인을 위협하다</t>
+  </si>
+  <si>
+    <t>테츠카브라(テツカブラ)의 혹 파괴</t>
   </si>
 </sst>
 </file>
@@ -3932,10 +3959,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J368"/>
+  <dimension ref="A1:J371"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A243" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="B324" sqref="B324"/>
+    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <pane ySplit="1" topLeftCell="A276" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B291" sqref="B291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15464,6 +15492,102 @@
         <v>441</v>
       </c>
     </row>
+    <row r="369" spans="1:10">
+      <c r="A369" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B369" t="s">
+        <v>1181</v>
+      </c>
+      <c r="C369" t="s">
+        <v>261</v>
+      </c>
+      <c r="D369" t="s">
+        <v>13</v>
+      </c>
+      <c r="E369" t="s">
+        <v>14</v>
+      </c>
+      <c r="F369" t="s">
+        <v>849</v>
+      </c>
+      <c r="G369" t="s">
+        <v>1182</v>
+      </c>
+      <c r="H369" t="s">
+        <v>268</v>
+      </c>
+      <c r="I369" t="s">
+        <v>69</v>
+      </c>
+      <c r="J369" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="370" spans="1:10">
+      <c r="A370" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B370" t="s">
+        <v>1184</v>
+      </c>
+      <c r="C370" t="s">
+        <v>381</v>
+      </c>
+      <c r="D370" t="s">
+        <v>13</v>
+      </c>
+      <c r="E370" t="s">
+        <v>14</v>
+      </c>
+      <c r="F370" t="s">
+        <v>382</v>
+      </c>
+      <c r="G370" t="s">
+        <v>1185</v>
+      </c>
+      <c r="H370" t="s">
+        <v>272</v>
+      </c>
+      <c r="I370" t="s">
+        <v>82</v>
+      </c>
+      <c r="J370" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="371" spans="1:10">
+      <c r="A371" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B371" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C371" t="s">
+        <v>381</v>
+      </c>
+      <c r="D371" t="s">
+        <v>13</v>
+      </c>
+      <c r="E371" t="s">
+        <v>14</v>
+      </c>
+      <c r="F371" t="s">
+        <v>477</v>
+      </c>
+      <c r="G371" t="s">
+        <v>1188</v>
+      </c>
+      <c r="H371" t="s">
+        <v>18</v>
+      </c>
+      <c r="I371" t="s">
+        <v>441</v>
+      </c>
+      <c r="J371" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J368" xr:uid="{864CE004-D11C-4921-BBE0-85FBA8C62B75}">
     <sortState ref="A2:J368">

</xml_diff>

<commit_message>
Completed translation of 'villagers' request'. Edit typo.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19007"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19024"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -1417,7 +1417,7 @@
     <t>ぽかぽかレスキュー隊出動！</t>
   </si>
   <si>
-    <t>폭신폭신레스큐대 출동!</t>
+    <t>따끈따끈 레스큐대 출동!</t>
   </si>
   <si>
     <t>이오스(イーオス) 12마리 토벌</t>
@@ -1555,7 +1555,7 @@
     <t>潜入！飛竜の巣！</t>
   </si>
   <si>
-    <t>잡입! 비룡의 둥지!</t>
+    <t>잠입! 비룡의 둥지!</t>
   </si>
   <si>
     <t>용의알(竜の卵) 2개 납품</t>
@@ -3274,7 +3274,7 @@
     <t>割り込み受注：卵納品</t>
   </si>
   <si>
-    <t>끼어들기 주의 : 알납품</t>
+    <t>새치기수주 : 알납품</t>
   </si>
   <si>
     <t>轟竜と赤甲獣のデュエット</t>
@@ -3962,8 +3962,8 @@
   <dimension ref="A1:J371"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="1" topLeftCell="A276" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B291" sqref="B291"/>
+      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>